<commit_message>
sort service names within each category
</commit_message>
<xml_diff>
--- a/AWS_Products.xlsx
+++ b/AWS_Products.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="460" windowWidth="33600" windowHeight="19760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="393">
   <si>
     <t>Category</t>
   </si>
@@ -834,13 +834,385 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/batch/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticbeanstalk/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/fargate/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lambda/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/serverless/serverlessrepo/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/autoscaling/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ecr/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/eks/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ecs/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lightsail/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/vmware/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowball-edge/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowball/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowmobile/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/storagegateway/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ebs/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/efs/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/glacier1/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/s3/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dms/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rds/aurora/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dynamodb/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticache/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/neptune/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rds/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/redshift/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/application-discovery/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/migration-hub/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/server-migration-service/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowball/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/directconnect/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/api-gateway/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudfront/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/route53/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/vpc/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticloadbalancing/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloud9/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codebuild/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codecommit/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codedeploy/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codepipeline/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codestar/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cli/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/xray/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/autoscaling/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudformation/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudtrail/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/config/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/opsworks/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/premiumsupport/phd/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/servicecatalog/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/systems-manager/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/trustedadvisor/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudwatch/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediaconvert/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/medialive/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediapackage/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediastore/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediatailor/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elastictranscoder/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kinesis/video-streams/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/certificate-manager/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudhsm/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/directoryservice/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iam/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kms/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/organizations/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/shield/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/single-sign-on/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/waf/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloud-directory/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cognito/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/guardduty/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/inspector/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/macie/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/datapipeline/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/glue/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/athena/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudsearch/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticmapreduce/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticsearch-service/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kinesis/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/quicksight/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/amazon-ai/amis/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/deeplens/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/comprehend/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lex/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/machine-learning/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/polly/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rekognition/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sagemaker/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/transcribe/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/translate/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mxnet/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/tensorflow/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/appsync/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/device-farm/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mobile/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mobile/sdk/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/pinpoint/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sumerian/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/step-functions/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/amazon-mq/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sns/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sqs/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/connect/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ses/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/alexaforbusiness/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/chime/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workdocs/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workmail/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/appstream2/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workspaces/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/greengrass/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-1-click/button/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-analytics/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot/button/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-core/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-device-defender/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-device-management/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/freertos/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/gamelift/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lumberyard/?p=tile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -858,6 +1230,22 @@
     <font>
       <u/>
       <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -881,16 +1269,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -900,10 +1292,30 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="16"/>
-        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -951,32 +1363,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -988,15 +1374,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D132" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D132" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:D132"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Category" dataDxfId="3"/>
-    <tableColumn id="3" name="AWS Service" dataDxfId="2"/>
-    <tableColumn id="4" name="Description" dataDxfId="1"/>
-    <tableColumn id="5" name="Link" dataDxfId="0" dataCellStyle="Hyperlink">
-      <calculatedColumnFormula>HYPERLINK(Table2[[#This Row],[Link]])</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" name="Category" dataDxfId="5"/>
+    <tableColumn id="3" name="AWS Service" dataDxfId="4"/>
+    <tableColumn id="4" name="Description" dataDxfId="3"/>
+    <tableColumn id="5" name="Link" dataDxfId="2" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1267,14 +1651,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="104.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1297,14 +1683,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/ec2/?p=tile</v>
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,14 +1697,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/ec2/autoscaling/?p=tile</v>
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1327,14 +1711,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/ecs/?p=tile</v>
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,14 +1725,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/eks/?p=tile</v>
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1357,14 +1739,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/ecr/?p=tile</v>
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1372,14 +1753,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/lightsail/?p=tile</v>
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,14 +1767,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/batch/?p=tile</v>
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,14 +1781,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/elasticbeanstalk/?p=tile</v>
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1417,14 +1795,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/fargate/?p=tile</v>
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,14 +1809,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/lambda/?p=tile</v>
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1447,14 +1823,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/serverless/serverlessrepo/?p=tile</v>
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1467,9 +1842,8 @@
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/vmware/?p=tile</v>
+      <c r="D13" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,14 +1851,13 @@
         <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/s3/?p=tile</v>
+        <v>42</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1492,14 +1865,13 @@
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/ebs/?p=tile</v>
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1507,14 +1879,13 @@
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/efs/?p=tile</v>
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,14 +1893,13 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/glacier1/?p=tile</v>
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1537,14 +1907,13 @@
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/storagegateway/?p=tile</v>
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,14 +1921,13 @@
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/snowball/?p=tile</v>
+        <v>34</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1567,14 +1935,13 @@
         <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/snowball-edge/?p=tile</v>
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1582,14 +1949,13 @@
         <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/snowmobile/?p=tile</v>
+        <v>30</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1597,14 +1963,13 @@
         <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/rds/aurora/?p=tile</v>
+        <v>59</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1612,14 +1977,13 @@
         <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/rds/?p=tile</v>
+        <v>47</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1632,9 +1996,8 @@
       <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/dynamodb/?hp=tile&amp;so-exp=below</v>
+      <c r="D24" s="2" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,9 +2010,8 @@
       <c r="C25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/elasticache/?p=tile</v>
+      <c r="D25" s="2" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1657,14 +2019,13 @@
         <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/redshift/?p=tile</v>
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1672,14 +2033,13 @@
         <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/neptune/?p=tile</v>
+        <v>49</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,14 +2047,13 @@
         <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/dms/?p=tile</v>
+        <v>55</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1707,9 +2066,8 @@
       <c r="C29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/application-discovery/?p=tile</v>
+      <c r="D29" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,9 +2080,8 @@
       <c r="C30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/dms/?p=tile</v>
+      <c r="D30" s="2" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,9 +2094,8 @@
       <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/migration-hub/?hp=tile&amp;so-exp=below</v>
+      <c r="D31" s="2" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1752,9 +2108,8 @@
       <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/server-migration-service/?p=tile</v>
+      <c r="D32" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1762,14 +2117,13 @@
         <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/snowball/?hp=tile&amp;so-exp=below</v>
+        <v>42</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1777,14 +2131,13 @@
         <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/snowball-edge/?p=tile</v>
+        <v>40</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1797,9 +2150,8 @@
       <c r="C35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/snowmobile/?p=tile</v>
+      <c r="D35" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,14 +2159,13 @@
         <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/vpc/?p=tile</v>
+        <v>77</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,14 +2173,13 @@
         <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloudfront/?p=tile</v>
+        <v>75</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1837,14 +2187,13 @@
         <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/route53/?p=tile</v>
+        <v>71</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1852,14 +2201,13 @@
         <v>67</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/api-gateway/?p=tile</v>
+        <v>73</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1867,14 +2215,13 @@
         <v>67</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/directconnect/?p=tile</v>
+        <v>69</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,9 +2234,8 @@
       <c r="C41" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/elasticloadbalancing/?p=tile</v>
+      <c r="D41" s="2" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,14 +2243,13 @@
         <v>80</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/codestar/?p=tile</v>
+        <v>92</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,14 +2257,13 @@
         <v>80</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/codecommit/?p=tile</v>
+        <v>86</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,14 +2271,13 @@
         <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/codebuild/?p=tile</v>
+        <v>84</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,9 +2290,8 @@
       <c r="C45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/codedeploy/?p=tile</v>
+      <c r="D45" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,9 +2304,8 @@
       <c r="C46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/codepipeline/?hp=tile&amp;so-exp=below</v>
+      <c r="D46" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,14 +2313,13 @@
         <v>80</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloud9/?p=tile</v>
+        <v>82</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1987,14 +2327,13 @@
         <v>80</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/xray/?p=tile</v>
+        <v>96</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2002,14 +2341,13 @@
         <v>80</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cli/?p=tile</v>
+        <v>94</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,14 +2355,13 @@
         <v>97</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloudwatch/?p=tile</v>
+        <v>101</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2032,14 +2369,13 @@
         <v>97</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D51" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/autoscaling/?p=tile</v>
+        <v>103</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2047,14 +2383,13 @@
         <v>97</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloudformation/?p=tile</v>
+        <v>105</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2062,14 +2397,13 @@
         <v>97</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D53" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloudtrail/?p=tile</v>
+        <v>107</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2077,14 +2411,13 @@
         <v>97</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D54" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/config/?p=tile</v>
+        <v>109</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,14 +2425,13 @@
         <v>97</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/opsworks/?p=tile</v>
+        <v>117</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,9 +2444,8 @@
       <c r="C56" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D56" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/servicecatalog/?p=tile</v>
+      <c r="D56" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2127,9 +2458,8 @@
       <c r="C57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D57" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/systems-manager/?p=tile</v>
+      <c r="D57" s="2" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,9 +2472,8 @@
       <c r="C58" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/trustedadvisor/?p=tile</v>
+      <c r="D58" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2152,14 +2481,13 @@
         <v>97</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D59" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/premiumsupport/phd/?p=tile</v>
+        <v>99</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,14 +2495,13 @@
         <v>118</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D60" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/elastictranscoder/?p=tile</v>
+        <v>124</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2182,14 +2509,13 @@
         <v>118</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D61" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/kinesis/video-streams/?p=tile</v>
+        <v>126</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,14 +2523,13 @@
         <v>118</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D62" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/mediaconvert/?p=tile</v>
+        <v>128</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,14 +2537,13 @@
         <v>118</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D63" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/medialive/?p=tile</v>
+        <v>130</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,14 +2551,13 @@
         <v>118</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D64" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/mediapackage/?p=tile</v>
+        <v>132</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2242,14 +2565,13 @@
         <v>118</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D65" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/mediastore/?p=tile</v>
+        <v>120</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2257,14 +2579,13 @@
         <v>118</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D66" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/mediatailor/?p=tile</v>
+        <v>122</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2272,14 +2593,13 @@
         <v>133</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D67" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/iam/?p=tile</v>
+        <v>149</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,14 +2607,13 @@
         <v>133</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D68" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloud-directory/?p=tile</v>
+        <v>151</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2302,14 +2621,13 @@
         <v>133</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cognito/?p=tile</v>
+        <v>77</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2317,14 +2635,13 @@
         <v>133</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/single-sign-on/?p=tile</v>
+        <v>153</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2332,14 +2649,13 @@
         <v>133</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D71" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/guardduty/?p=tile</v>
+        <v>135</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2347,14 +2663,13 @@
         <v>133</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>76</v>
+        <v>154</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D72" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/directconnect/?p=tile</v>
+        <v>155</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2362,14 +2677,13 @@
         <v>133</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D73" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/inspector/?p=tile</v>
+        <v>157</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2377,14 +2691,13 @@
         <v>133</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D74" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/macie/?hp=tile&amp;so-exp=below</v>
+        <v>159</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2392,14 +2705,13 @@
         <v>133</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D75" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/certificate-manager/?p=tile</v>
+        <v>141</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2407,14 +2719,13 @@
         <v>133</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D76" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloudhsm/?p=tile</v>
+        <v>161</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,14 +2733,13 @@
         <v>133</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D77" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/directoryservice/?p=tile</v>
+        <v>137</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2437,14 +2747,13 @@
         <v>133</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D78" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/kms/?p=tile</v>
+        <v>139</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2452,14 +2761,13 @@
         <v>133</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D79" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/organizations/?p=tile</v>
+        <v>143</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2467,14 +2775,13 @@
         <v>133</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D80" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/shield/?p=tile</v>
+        <v>145</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2482,14 +2789,13 @@
         <v>133</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D81" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/waf/?p=tile</v>
+        <v>147</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,14 +2803,13 @@
         <v>162</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D82" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/athena/?p=tile</v>
+        <v>176</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2512,14 +2817,13 @@
         <v>162</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D83" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/elasticmapreduce/?p=tile</v>
+        <v>178</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2527,14 +2831,13 @@
         <v>162</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D84" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/cloudsearch/?p=tile</v>
+        <v>164</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2542,14 +2845,13 @@
         <v>162</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D85" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/elasticsearch-service/?p=tile</v>
+        <v>168</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2557,14 +2859,13 @@
         <v>162</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D86" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/kinesis/?p=tile</v>
+        <v>166</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2572,14 +2873,13 @@
         <v>162</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D87" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/redshift/?p=tile</v>
+        <v>170</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2587,14 +2887,13 @@
         <v>162</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D88" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/quicksight/?p=tile</v>
+        <v>172</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2602,14 +2901,13 @@
         <v>162</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D89" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/datapipeline/?p=tile</v>
+        <v>174</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2617,14 +2915,13 @@
         <v>162</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>177</v>
+        <v>54</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D90" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/glue/?p=tile</v>
+        <v>55</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2632,14 +2929,13 @@
         <v>179</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D91" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/sagemaker/?p=tile</v>
+        <v>199</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2647,14 +2943,13 @@
         <v>179</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D92" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/comprehend/?p=tile</v>
+        <v>197</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2662,14 +2957,13 @@
         <v>179</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D93" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/lex/?p=tile</v>
+        <v>183</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2677,14 +2971,13 @@
         <v>179</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D94" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/polly/?p=tile</v>
+        <v>185</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2692,14 +2985,13 @@
         <v>179</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D95" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/rekognition/?p=tile</v>
+        <v>191</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2707,14 +2999,13 @@
         <v>179</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D96" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/machine-learning/?p=tile</v>
+        <v>187</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2722,14 +3013,13 @@
         <v>179</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D97" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/translate/?p=tile</v>
+        <v>189</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2737,14 +3027,13 @@
         <v>179</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D98" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/transcribe/?p=tile</v>
+        <v>181</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2752,14 +3041,13 @@
         <v>179</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D99" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/deeplens/?p=tile</v>
+        <v>195</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2767,14 +3055,13 @@
         <v>179</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D100" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/amazon-ai/amis/?p=tile</v>
+        <v>193</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2787,9 +3074,8 @@
       <c r="C101" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D101" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/mxnet/?p=tile</v>
+      <c r="D101" s="2" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2802,9 +3088,8 @@
       <c r="C102" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D102" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/tensorflow/?p=tile</v>
+      <c r="D102" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2812,14 +3097,13 @@
         <v>204</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D103" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/mobile/?p=tile</v>
+        <v>210</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2827,14 +3111,13 @@
         <v>204</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D104" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/api-gateway/?p=tile</v>
+        <v>212</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2842,14 +3125,13 @@
         <v>204</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D105" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/pinpoint/?p=tile</v>
+        <v>206</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2857,14 +3139,13 @@
         <v>204</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D106" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/appsync/?p=tile</v>
+        <v>214</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2872,14 +3153,13 @@
         <v>204</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>211</v>
+        <v>74</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D107" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/device-farm/?p=tile</v>
+        <v>75</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2887,14 +3167,13 @@
         <v>204</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D108" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/mobile/sdk/?p=tile</v>
+        <v>208</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,9 +3186,8 @@
       <c r="C109" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D109" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/sumerian/?p=tile</v>
+      <c r="D109" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2922,9 +3200,8 @@
       <c r="C110" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D110" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/step-functions/?p=tile</v>
+      <c r="D110" s="2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2932,14 +3209,13 @@
         <v>218</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D111" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/sqs/?p=tile</v>
+        <v>226</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2952,9 +3228,8 @@
       <c r="C112" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D112" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/sns/?p=tile</v>
+      <c r="D112" s="2" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2962,14 +3237,13 @@
         <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D113" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/amazon-mq/?p=tile</v>
+        <v>222</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2982,9 +3256,8 @@
       <c r="C114" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D114" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/connect/?p=tile</v>
+      <c r="D114" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2997,9 +3270,8 @@
       <c r="C115" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D115" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/pinpoint/?p=tile</v>
+      <c r="D115" s="2" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,9 +3284,8 @@
       <c r="C116" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D116" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/ses/?p=tile</v>
+      <c r="D116" s="2" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3027,9 +3298,8 @@
       <c r="C117" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D117" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/alexaforbusiness/?p=tile</v>
+      <c r="D117" s="2" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3042,9 +3312,8 @@
       <c r="C118" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D118" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/chime/?p=tile</v>
+      <c r="D118" s="2" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3057,9 +3326,8 @@
       <c r="C119" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D119" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/workdocs/?p=tile</v>
+      <c r="D119" s="2" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3072,9 +3340,8 @@
       <c r="C120" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D120" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/workmail/?p=tile</v>
+      <c r="D120" s="2" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3082,14 +3349,13 @@
         <v>241</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D121" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/workspaces/?hp=tile&amp;so-exp=below</v>
+        <v>245</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3097,14 +3363,13 @@
         <v>241</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D122" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/appstream2/?hp=tile&amp;so-exp=below</v>
+        <v>243</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3112,14 +3377,13 @@
         <v>246</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D123" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/iot-core/?p=tile</v>
+        <v>252</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3127,14 +3391,13 @@
         <v>246</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D124" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/freertos/?p=tile</v>
+        <v>254</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3142,14 +3405,13 @@
         <v>246</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D125" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/greengrass/?p=tile</v>
+        <v>256</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3157,14 +3419,13 @@
         <v>246</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D126" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/iot-1-click/button/?p=tile</v>
+        <v>258</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3172,14 +3433,13 @@
         <v>246</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D127" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/iot-analytics/?p=tile</v>
+        <v>248</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3187,14 +3447,13 @@
         <v>246</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D128" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/iot/button/?p=tile</v>
+        <v>260</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3202,14 +3461,13 @@
         <v>246</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D129" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/iot-device-defender/?p=tile</v>
+        <v>262</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3217,14 +3475,13 @@
         <v>246</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D130" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/iot-device-management/?p=tile</v>
+        <v>250</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3237,9 +3494,8 @@
       <c r="C131" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D131" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/gamelift/?p=tile</v>
+      <c r="D131" s="2" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3252,13 +3508,13 @@
       <c r="C132" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D132" s="2" t="str">
-        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
-        <v>https://aws.amazon.com/lumberyard/?p=tile</v>
+      <c r="D132" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
updated the csv and xlsx files
</commit_message>
<xml_diff>
--- a/AWS_Products.xlsx
+++ b/AWS_Products.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palsarma/git/github/palsarma/aws_products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{52778237-077E-F44F-BDA0-61A7630AA219}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A6CC1A1E-DC28-A841-B7A5-638AE4C32049}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="424">
   <si>
     <t>Category</t>
   </si>
@@ -771,9 +771,6 @@
     <t>https://aws.amazon.com/storagegateway/?nc2=h_l3_sc</t>
   </si>
   <si>
-    <t>Amazon Elastic Block Storage (EBS)</t>
-  </si>
-  <si>
     <t>EC2 Block Storage Volumes</t>
   </si>
   <si>
@@ -891,9 +888,6 @@
     <t>Tools and SDKs for AWS</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/getting-started/resource-center/tools-sdks/?nc2=h_l3_dm</t>
-  </si>
-  <si>
     <t>https://aws.amazon.com/xray/?nc2=h_l3_dm</t>
   </si>
   <si>
@@ -1041,9 +1035,6 @@
     <t>Deep Learning on Amazon EC2</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/amazon-ai/amis/?nc2=h_l3_al</t>
-  </si>
-  <si>
     <t>https://aws.amazon.com/deeplens/?nc2=h_l3_al</t>
   </si>
   <si>
@@ -1128,15 +1119,9 @@
     <t>Build, Test, and Monitor Mobile Apps</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/mobilehub/?nc2=h_l3_as</t>
-  </si>
-  <si>
     <t>Build High Quality Mobile Apps Quickly and Easily</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/mobile/sdk/?nc2=h_l3_ms</t>
-  </si>
-  <si>
     <t>User Identity and App Data Synchronization</t>
   </si>
   <si>
@@ -1288,6 +1273,33 @@
   </si>
   <si>
     <t>https://aws.amazon.com/quicksight/</t>
+  </si>
+  <si>
+    <t>Amazon Elastic Block Store (EBS)</t>
+  </si>
+  <si>
+    <t>Amazon VPC PrivateLink</t>
+  </si>
+  <si>
+    <t>Securely access services hosted on AWS</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/privatelink/?nc2=h_l3_n</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/getting-started/tools-sdks/?nc2=h_l3_dm</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/machine-learning/amis/?nc2=h_l3_al</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mobile/?nc2=h_l3_as</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mobile/resources/?nc2=h_l3_ms</t>
+  </si>
+  <si>
+    <t>LinkText</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1372,26 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1429,13 +1460,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D142" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:D142" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AWS Service" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Link" dataCellStyle="Hyperlink"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E143" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E143" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AWS Service" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LinkText" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{F37A6230-26FE-F443-B93E-E500764AE6AC}" name="Link" dataDxfId="0">
+      <calculatedColumnFormula>HYPERLINK(D2,D2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1704,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1715,11 +1749,12 @@
     <col min="1" max="1" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="82.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="82.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1730,10 +1765,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1746,8 +1784,12 @@
       <c r="D2" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="str">
+        <f t="shared" ref="D2:E33" si="0">HYPERLINK(D2,D2)</f>
+        <v>https://aws.amazon.com/batch/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1760,8 +1802,12 @@
       <c r="D3" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/elasticbeanstalk/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1774,8 +1820,12 @@
       <c r="D4" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/fargate/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1788,8 +1838,12 @@
       <c r="D5" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/lambda/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1802,8 +1856,12 @@
       <c r="D6" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/serverless/serverlessrepo/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1816,8 +1874,12 @@
       <c r="D7" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/ec2/autoscaling/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1830,8 +1892,12 @@
       <c r="D8" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/ec2/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1844,8 +1910,12 @@
       <c r="D9" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/ecr/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1858,8 +1928,12 @@
       <c r="D10" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/eks/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1872,8 +1946,12 @@
       <c r="D11" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/ecs/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1884,10 +1962,14 @@
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/lightsail/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1900,8 +1982,12 @@
       <c r="D13" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/vmware/?nc2=h_l3_n</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1914,8 +2000,12 @@
       <c r="D14" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/snowball-edge/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1928,8 +2018,12 @@
       <c r="D15" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/snowball/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1942,8 +2036,12 @@
       <c r="D16" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/snowmobile/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1956,36 +2054,48 @@
       <c r="D17" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/storagegateway/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
+        <v>415</v>
+      </c>
+      <c r="C18" t="s">
         <v>247</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/ebs/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
+        <v>249</v>
+      </c>
+      <c r="C19" t="s">
         <v>250</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/efs/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1996,26 +2106,34 @@
         <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="E20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/glacier/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/s3/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>256</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
@@ -2024,12 +2142,16 @@
         <v>49</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="E22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/dms/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
@@ -2038,12 +2160,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="E23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/rds/aurora/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
@@ -2052,26 +2178,34 @@
         <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="E24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/dynamodb/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
       </c>
       <c r="C25" t="s">
+        <v>259</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/elasticache/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
@@ -2080,12 +2214,16 @@
         <v>47</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="E26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/neptune/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
@@ -2094,24 +2232,32 @@
         <v>40</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="E27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/rds/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
       </c>
       <c r="C28" t="s">
+        <v>263</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/redshift/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -2119,13 +2265,17 @@
         <v>51</v>
       </c>
       <c r="C29" t="s">
+        <v>265</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/application-discovery/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -2136,10 +2286,14 @@
         <v>49</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="E30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/dms/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -2150,10 +2304,14 @@
         <v>53</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+      <c r="E31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/migration-hub/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -2161,13 +2319,17 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
+        <v>268</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/server-migration-service/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -2180,8 +2342,12 @@
       <c r="D33" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://aws.amazon.com/snowball-edge/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -2194,8 +2360,12 @@
       <c r="D34" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="str">
+        <f t="shared" ref="D34:E65" si="1">HYPERLINK(D34,D34)</f>
+        <v>https://aws.amazon.com/snowball/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -2208,8 +2378,12 @@
       <c r="D35" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/snowmobile/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -2220,10 +2394,14 @@
         <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="E36" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/directconnect/?nc2=h_l3_n</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -2234,10 +2412,14 @@
         <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="E37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/api-gateway/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -2248,10 +2430,14 @@
         <v>59</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+      <c r="E38" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/cloudfront/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2259,1452 +2445,1886 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
+        <v>273</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/route53/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
       <c r="B40" t="s">
+        <v>416</v>
+      </c>
+      <c r="C40" t="s">
+        <v>417</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/privatelink/?nc2=h_l3_n</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>76</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+      <c r="E41" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/vpc/?nc2=h_l3_n</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="E42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/cloud9/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="E43" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/codebuild/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>65</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="E44" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/codecommit/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>279</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="E45" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/codedeploy/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="E46" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/codepipeline/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="E47" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/codestar/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>65</v>
       </c>
       <c r="B48" t="s">
-        <v>285</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
-        <v>286</v>
+        <v>80</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+      <c r="E48" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/cli/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>65</v>
       </c>
       <c r="B49" t="s">
+        <v>284</v>
+      </c>
+      <c r="C49" t="s">
+        <v>285</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E49" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/getting-started/tools-sdks/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" t="s">
-        <v>85</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="E50" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/xray/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+      <c r="E51" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/autoscaling/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>81</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="E52" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/cloudformation/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>81</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="E53" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/cloudtrail/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+      <c r="E54" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/cli/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>294</v>
+        <v>91</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="E55" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/config/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C56" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="E56" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/managed-services/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>92</v>
+        <v>294</v>
       </c>
       <c r="C57" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="E57" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/console/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="E58" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/opsworks/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>81</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>299</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="E59" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/premiumsupport/phd/?nc2=h_l3_mt</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C60" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+      <c r="E60" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/servicecatalog/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>81</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="E61" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/systems-manager/?nc2=h_l3_mt</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>81</v>
       </c>
       <c r="B62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E62" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/premiumsupport/trustedadvisor/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" t="s">
         <v>82</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>100</v>
-      </c>
-      <c r="B63" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" t="s">
-        <v>106</v>
-      </c>
       <c r="D63" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="E63" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/cloudwatch/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>100</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+      <c r="E64" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/mediaconvert/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>100</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+      <c r="E65" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://aws.amazon.com/medialive/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>100</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+      <c r="E66" s="2" t="str">
+        <f t="shared" ref="D66:E97" si="2">HYPERLINK(D66,D66)</f>
+        <v>https://aws.amazon.com/mediapackage/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="E67" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/mediastore/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>100</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C68" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="E68" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/mediatailor/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>100</v>
       </c>
       <c r="B69" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" t="s">
+        <v>102</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E69" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/elastictranscoder/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" t="s">
         <v>103</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>104</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>115</v>
-      </c>
-      <c r="B70" t="s">
-        <v>128</v>
-      </c>
-      <c r="C70" t="s">
-        <v>129</v>
-      </c>
       <c r="D70" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+      <c r="E70" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/kinesis/video-streams/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>115</v>
       </c>
       <c r="B71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="E71" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/certificate-manager/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>115</v>
       </c>
       <c r="B72" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="E72" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/cloudhsm/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>115</v>
       </c>
       <c r="B73" t="s">
-        <v>317</v>
+        <v>132</v>
       </c>
       <c r="C73" t="s">
-        <v>318</v>
+        <v>133</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+      <c r="E73" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/directoryservice/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C74" t="s">
-        <v>116</v>
+        <v>316</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="E74" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/firewall-manager/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>134</v>
+        <v>318</v>
       </c>
       <c r="C75" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="E75" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/iam/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C76" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="E76" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/kms/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>324</v>
+        <v>136</v>
       </c>
       <c r="C77" t="s">
-        <v>325</v>
+        <v>137</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="E77" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/organizations/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>138</v>
+        <v>322</v>
       </c>
       <c r="C78" t="s">
-        <v>139</v>
+        <v>323</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="E78" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/secrets-manager/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>115</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C79" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+      <c r="E79" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/shield/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>115</v>
       </c>
       <c r="B80" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="C80" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+      <c r="E80" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/single-sign-on/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>115</v>
       </c>
       <c r="B81" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="C81" t="s">
-        <v>330</v>
+        <v>141</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+      <c r="E81" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/waf/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>115</v>
       </c>
       <c r="B82" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
-        <v>119</v>
+        <v>328</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="E82" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/cloud-directory/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>115</v>
       </c>
       <c r="B83" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="E83" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/cognito/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>115</v>
       </c>
       <c r="B84" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+      <c r="E84" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/guardduty/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>115</v>
       </c>
       <c r="B85" t="s">
+        <v>124</v>
+      </c>
+      <c r="C85" t="s">
+        <v>125</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E85" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/inspector/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" t="s">
         <v>126</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>127</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>156</v>
-      </c>
-      <c r="B86" t="s">
-        <v>175</v>
-      </c>
-      <c r="C86" t="s">
-        <v>336</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+      <c r="E86" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/macie/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>156</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C87" t="s">
-        <v>174</v>
+        <v>334</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+      <c r="E87" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/machine-learning/amis/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>156</v>
       </c>
       <c r="B88" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="C88" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="E88" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/deeplens/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>156</v>
       </c>
       <c r="B89" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C89" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+      <c r="E89" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/comprehend/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>156</v>
       </c>
       <c r="B90" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C90" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+      <c r="E90" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/lex/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>156</v>
       </c>
       <c r="B91" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C91" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+      <c r="E91" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/aml/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>156</v>
       </c>
       <c r="B92" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C92" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="E92" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/polly/?nc2=h_l3_c</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>156</v>
       </c>
       <c r="B93" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C93" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+      <c r="E93" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/rekognition/?nc2=h_l3_sc</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>156</v>
       </c>
       <c r="B94" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C94" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+      <c r="E94" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/sagemaker/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>156</v>
       </c>
       <c r="B95" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C95" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="E95" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/transcribe/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>156</v>
       </c>
       <c r="B96" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C96" t="s">
-        <v>347</v>
+        <v>170</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="E96" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/translate/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>156</v>
       </c>
       <c r="B97" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" t="s">
+        <v>344</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E97" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>https://aws.amazon.com/mxnet/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>156</v>
+      </c>
+      <c r="B98" t="s">
         <v>177</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>178</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>142</v>
-      </c>
-      <c r="B98" t="s">
-        <v>153</v>
-      </c>
-      <c r="C98" t="s">
-        <v>350</v>
-      </c>
       <c r="D98" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+      <c r="E98" s="2" t="str">
+        <f t="shared" ref="D98:E129" si="3">HYPERLINK(D98,D98)</f>
+        <v>https://aws.amazon.com/tensorflow/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>142</v>
       </c>
       <c r="B99" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C99" t="s">
-        <v>155</v>
+        <v>347</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="E99" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/datapipeline/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>142</v>
       </c>
       <c r="B100" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="C100" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+      <c r="E100" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/glue/?nc2=h_l3_an</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>142</v>
       </c>
       <c r="B101" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C101" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+      <c r="E101" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/athena/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>142</v>
       </c>
       <c r="B102" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C102" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="E102" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/cloudsearch/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>142</v>
       </c>
       <c r="B103" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C103" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="E103" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/emr/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>142</v>
       </c>
       <c r="B104" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C104" t="s">
-        <v>357</v>
+        <v>150</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="E104" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/elasticsearch-service/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>142</v>
       </c>
       <c r="B105" t="s">
-        <v>359</v>
+        <v>151</v>
       </c>
       <c r="C105" t="s">
-        <v>152</v>
+        <v>354</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="E105" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/kinesis/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>142</v>
       </c>
       <c r="B106" t="s">
+        <v>356</v>
+      </c>
+      <c r="C106" t="s">
+        <v>152</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E106" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/quicksight/</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>142</v>
+      </c>
+      <c r="B107" t="s">
         <v>44</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>45</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>179</v>
-      </c>
-      <c r="B107" t="s">
-        <v>183</v>
-      </c>
-      <c r="C107" t="s">
-        <v>361</v>
-      </c>
       <c r="D107" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+      <c r="E107" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/redshift/?nc2=h_l3_al</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>179</v>
       </c>
       <c r="B108" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C108" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="E108" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/appsync/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>179</v>
       </c>
       <c r="B109" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C109" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+      <c r="E109" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/device-farm/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>179</v>
       </c>
       <c r="B110" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C110" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+      <c r="E110" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/mobile/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>179</v>
       </c>
       <c r="B111" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="C111" t="s">
-        <v>62</v>
+        <v>363</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+      <c r="E111" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/mobile/resources/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>179</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
+        <v>61</v>
       </c>
       <c r="C112" t="s">
-        <v>369</v>
+        <v>62</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="E112" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/api-gateway/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>179</v>
       </c>
       <c r="B113" t="s">
+        <v>118</v>
+      </c>
+      <c r="C113" t="s">
+        <v>364</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E113" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/cognito/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>179</v>
+      </c>
+      <c r="B114" t="s">
         <v>181</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>182</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="D114" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E114" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/pinpoint/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>186</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>187</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>188</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>189</v>
-      </c>
-      <c r="B115" t="s">
-        <v>183</v>
-      </c>
-      <c r="C115" t="s">
-        <v>361</v>
-      </c>
       <c r="D115" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+      <c r="E115" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/sumerian/?nc2=h_l3_db</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>189</v>
       </c>
       <c r="B116" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C116" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="E116" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/appsync/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>189</v>
       </c>
       <c r="B117" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C117" t="s">
-        <v>196</v>
+        <v>367</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+      <c r="E117" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/step-functions/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>189</v>
       </c>
       <c r="B118" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C118" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+      <c r="E118" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/amazon-mq/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>189</v>
       </c>
       <c r="B119" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" t="s">
+        <v>194</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E119" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/sns/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>189</v>
+      </c>
+      <c r="B120" t="s">
         <v>191</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>192</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>197</v>
-      </c>
-      <c r="B120" t="s">
-        <v>198</v>
-      </c>
-      <c r="C120" t="s">
-        <v>377</v>
-      </c>
       <c r="D120" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="E120" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/sqs/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>197</v>
       </c>
       <c r="B121" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="C121" t="s">
-        <v>182</v>
+        <v>372</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+      <c r="E121" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/connect/?nc2=h_l3_cc</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>197</v>
       </c>
       <c r="B122" t="s">
+        <v>181</v>
+      </c>
+      <c r="C122" t="s">
+        <v>182</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E122" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/pinpoint/?nc2=h_l3_ms</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>197</v>
+      </c>
+      <c r="B123" t="s">
         <v>199</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" t="s">
         <v>200</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>201</v>
-      </c>
-      <c r="B123" t="s">
-        <v>202</v>
-      </c>
-      <c r="C123" t="s">
-        <v>380</v>
-      </c>
       <c r="D123" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+      <c r="E123" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/ses/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>201</v>
       </c>
       <c r="B124" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C124" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+      <c r="E124" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/alexaforbusiness/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>201</v>
       </c>
       <c r="B125" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C125" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+      <c r="E125" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/chime/</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>201</v>
       </c>
       <c r="B126" t="s">
+        <v>204</v>
+      </c>
+      <c r="C126" t="s">
+        <v>379</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E126" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/workdocs/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>201</v>
+      </c>
+      <c r="B127" t="s">
         <v>205</v>
       </c>
-      <c r="C126" t="s">
-        <v>386</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>206</v>
-      </c>
-      <c r="B127" t="s">
-        <v>208</v>
-      </c>
       <c r="C127" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+      <c r="E127" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/workmail/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>206</v>
       </c>
       <c r="B128" t="s">
+        <v>208</v>
+      </c>
+      <c r="C128" t="s">
+        <v>383</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E128" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/appstream2/?nc2=h_l3_as</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>206</v>
+      </c>
+      <c r="B129" t="s">
         <v>207</v>
       </c>
-      <c r="C128" t="s">
-        <v>390</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>209</v>
-      </c>
-      <c r="B129" t="s">
-        <v>214</v>
-      </c>
       <c r="C129" t="s">
-        <v>215</v>
+        <v>385</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="E129" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>https://aws.amazon.com/workspaces/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>209</v>
       </c>
       <c r="B130" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C130" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="E130" s="2" t="str">
+        <f t="shared" ref="D130:E161" si="4">HYPERLINK(D130,D130)</f>
+        <v>https://aws.amazon.com/greengrass/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>209</v>
       </c>
       <c r="B131" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C131" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="E131" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/iot-1-click/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>209</v>
       </c>
       <c r="B132" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C132" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+      <c r="E132" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/iot-analytics/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>209</v>
       </c>
       <c r="B133" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="C133" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="E133" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/iotbutton/</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>209</v>
       </c>
       <c r="B134" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C134" t="s">
-        <v>397</v>
+        <v>211</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+      <c r="E134" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/iot-core/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>209</v>
       </c>
       <c r="B135" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C135" t="s">
-        <v>224</v>
+        <v>392</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+      <c r="E135" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/iot-device-defender/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>209</v>
       </c>
       <c r="B136" t="s">
+        <v>223</v>
+      </c>
+      <c r="C136" t="s">
+        <v>224</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E136" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/iot-device-management/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>209</v>
+      </c>
+      <c r="B137" t="s">
         <v>212</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>213</v>
       </c>
-      <c r="D136" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>225</v>
-      </c>
-      <c r="B137" t="s">
-        <v>226</v>
-      </c>
-      <c r="C137" t="s">
-        <v>401</v>
-      </c>
       <c r="D137" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+      <c r="E137" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/freertos/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>225</v>
       </c>
       <c r="B138" t="s">
+        <v>226</v>
+      </c>
+      <c r="C138" t="s">
+        <v>396</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E138" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/gamelift/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>225</v>
+      </c>
+      <c r="B139" t="s">
         <v>227</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C139" t="s">
+        <v>398</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E139" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/lumberyard/?nc2=h_l3_ap</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>400</v>
+      </c>
+      <c r="B140" t="s">
+        <v>401</v>
+      </c>
+      <c r="C140" t="s">
+        <v>402</v>
+      </c>
+      <c r="D140" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="D138" s="2" t="s">
+      <c r="E140" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/aws-cost-management/aws-budgets/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>400</v>
+      </c>
+      <c r="B141" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="C141" t="s">
         <v>405</v>
       </c>
-      <c r="B139" t="s">
+      <c r="D141" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C139" t="s">
+      <c r="E141" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/aws-cost-management/aws-cost-explorer/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>400</v>
+      </c>
+      <c r="B142" t="s">
         <v>407</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="C142" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>405</v>
-      </c>
-      <c r="B140" t="s">
+      <c r="D142" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="C140" t="s">
+      <c r="E142" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/aws-cost-management/aws-cost-and-usage-reporting/?nc2=h_l3_dm</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>400</v>
+      </c>
+      <c r="B143" t="s">
         <v>410</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="C143" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>405</v>
-      </c>
-      <c r="B141" t="s">
+      <c r="D143" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C141" t="s">
-        <v>413</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>405</v>
-      </c>
-      <c r="B142" t="s">
-        <v>415</v>
-      </c>
-      <c r="C142" t="s">
-        <v>416</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>417</v>
+      <c r="E143" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>https://aws.amazon.com/aws-cost-management/reserved-instance-reporting/?nc2=h_l3_dm</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to keep up with AWS Products page changes
</commit_message>
<xml_diff>
--- a/AWS_Products.xlsx
+++ b/AWS_Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palsarma/git/github/palsarma/aws_products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A6CC1A1E-DC28-A841-B7A5-638AE4C32049}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AD0D25F1-43F4-4849-ABE5-89B53CE68ABC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="406">
   <si>
     <t>Category</t>
   </si>
@@ -717,589 +717,535 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/batch/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elasticbeanstalk/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>Run Containers Without Managing Servers or Clusters</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/fargate/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>Run Code without Thinking about Servers</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/lambda/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/serverless/serverlessrepo/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/autoscaling/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ecr/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/eks/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ecs/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>Build a Hybrid Cloud Without Custom Hardware</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/vmware/?nc2=h_l3_n</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowball-edge/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowball/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowmobile/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/storagegateway/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>EC2 Block Storage Volumes</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ebs/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>Amazon Elastic File System (EFS)</t>
-  </si>
-  <si>
-    <t>Fully Managed File System for EC2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/efs/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/glacier/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>Amazon Simple Storage Service (S3)</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/s3/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/dms/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/rds/aurora/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/dynamodb/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>In-memory Caching Service</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elasticache/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/neptune/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/rds/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>Fast, Simple, Cost-Effective Data Warehousing</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/redshift/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>Discover on-premises applications to streamline migration</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/application-discovery/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/migration-hub/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>Migrate On-premises servers to AWS</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/server-migration-service/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/directconnect/?nc2=h_l3_n</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/api-gateway/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudfront/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>Scalable Domain Name System (DNS)</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/route53/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/vpc/?nc2=h_l3_n</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloud9/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codebuild/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codecommit/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>Automate Code Deployments</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codedeploy/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codepipeline/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codestar/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cli/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>AWS Tools &amp; SDKs</t>
-  </si>
-  <si>
-    <t>Tools and SDKs for AWS</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/xray/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/autoscaling/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudformation/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudtrail/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/config/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>AWS Managed Services</t>
-  </si>
-  <si>
-    <t>Infrastructure Operations Management for AWS</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/managed-services/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>AWS Management Console</t>
-  </si>
-  <si>
-    <t>Web-based User Interface</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/console/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>Automate operations with Chef and Puppet</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/opsworks/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>Personalized view of AWS service health</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/premiumsupport/phd/?nc2=h_l3_mt</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/servicecatalog/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/systems-manager/?nc2=h_l3_mt</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/premiumsupport/trustedadvisor/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudwatch/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediaconvert/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/medialive/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediapackage/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediastore/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediatailor/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elastictranscoder/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/kinesis/video-streams/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/certificate-manager/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudhsm/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/directoryservice/?nc2=h_l3_dm</t>
-  </si>
-  <si>
     <t>AWS Firewall Manager</t>
   </si>
   <si>
     <t>Central Management of Firewall Rules</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/firewall-manager/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>AWS Identity and Access Management (IAM)</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iam/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/kms/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/organizations/?nc2=h_l3_dm</t>
-  </si>
-  <si>
     <t>AWS Secrets Manager</t>
   </si>
   <si>
     <t>Rotate, Manage, and Retrieve Secrets</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/secrets-manager/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/shield/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/single-sign-on/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/waf/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>Create Flexible Cloud-Native Directories</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloud-directory/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cognito/?nc2=h_l3_ms</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/guardduty/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/inspector/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/macie/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>Deep Learning on Amazon EC2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/deeplens/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/comprehend/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/lex/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/aml/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/polly/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/rekognition/?nc2=h_l3_sc</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sagemaker/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/transcribe/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/translate/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>Scalable, Open-source Deep Learning Framework</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mxnet/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/tensorflow/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>Orchestration Service for Periodic, Data-Driven Workflows</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/datapipeline/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/glue/?nc2=h_l3_an</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/athena/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudsearch/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/emr/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elasticsearch-service/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>Analyze Real-time Video and Data Streams</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/kinesis/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>Amazon QuickSight</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/redshift/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>Real-Time and Offline Mobile Data Apps</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/appsync/?nc2=h_l3_ms</t>
-  </si>
-  <si>
-    <t>Test Android, iOS, and Web Apps on Real Devices in the AWS Cloud</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/device-farm/?nc2=h_l3_ms</t>
-  </si>
-  <si>
-    <t>Build, Test, and Monitor Mobile Apps</t>
-  </si>
-  <si>
-    <t>Build High Quality Mobile Apps Quickly and Easily</t>
-  </si>
-  <si>
-    <t>User Identity and App Data Synchronization</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/pinpoint/?nc2=h_l3_ms</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sumerian/?nc2=h_l3_db</t>
-  </si>
-  <si>
-    <t>Coordination for Distributed Applications</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/step-functions/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/amazon-mq/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sns/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sqs/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>Cloud-Based Contact Center Service</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/connect/?nc2=h_l3_cc</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ses/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>Empower Your Organization with Alexa</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/alexaforbusiness/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>Frustration-free meetings, video calls, and chat</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/chime/</t>
-  </si>
-  <si>
-    <t>Secure Enterprise Document Storage and Sharing</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/workdocs/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>Secure Email and Calendaring</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/workmail/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>Stream desktop applications securely to a browser</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/appstream2/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>Virtual Desktops in the Cloud</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/workspaces/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/greengrass/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-1-click/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-analytics/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iotbutton/</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-core/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>Security Management for IoT Devices</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-device-defender/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-device-management/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/freertos/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>Amazon GameLift: Simple, fast, cost-effective dedicated game server hosting.</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/gamelift/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>A Free Cross-Platform 3D Game Engine, with Full Source, Integrated with AWS and Twitch</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/lumberyard/?nc2=h_l3_ap</t>
-  </si>
-  <si>
-    <t>AWS Cost Management</t>
-  </si>
-  <si>
-    <t>AWS Budgets</t>
-  </si>
-  <si>
-    <t>Set Custom Cost and Usage Budgets</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/aws-cost-management/aws-budgets/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>AWS Cost Explorer</t>
-  </si>
-  <si>
-    <t>Analyze Your AWS Cost and Usage</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/aws-cost-management/aws-cost-explorer/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>AWS Cost and Usage Report</t>
-  </si>
-  <si>
-    <t>Access Comprehensive Cost and Usage Information</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/aws-cost-management/aws-cost-and-usage-reporting/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>Reserved Instance Reporting</t>
-  </si>
-  <si>
-    <t>Dive Deeper into Your Reserved Instances (RIs)</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/aws-cost-management/reserved-instance-reporting/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/lightsail/?nc2=h_l3_c</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/quicksight/</t>
-  </si>
-  <si>
-    <t>Amazon Elastic Block Store (EBS)</t>
-  </si>
-  <si>
     <t>Amazon VPC PrivateLink</t>
   </si>
   <si>
     <t>Securely access services hosted on AWS</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/privatelink/?nc2=h_l3_n</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/getting-started/tools-sdks/?nc2=h_l3_dm</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/machine-learning/amis/?nc2=h_l3_al</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mobile/?nc2=h_l3_as</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mobile/resources/?nc2=h_l3_ms</t>
-  </si>
-  <si>
     <t>LinkText</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/batch/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticbeanstalk/?p=tile</t>
+  </si>
+  <si>
+    <t>Run Containers without Managing Servers or Clusters</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/fargate/?p=tile</t>
+  </si>
+  <si>
+    <t>Run your Code in Response to Events</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lambda/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/serverless/serverlessrepo/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/autoscaling/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ecr/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/eks/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ecs/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lightsail/?p=tile</t>
+  </si>
+  <si>
+    <t>Build a Hybrid Cloud without Custom Hardware</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/vmware/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowball-edge/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowball/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowmobile/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/storagegateway/?p=tile</t>
+  </si>
+  <si>
+    <t>Amazon EBS</t>
+  </si>
+  <si>
+    <t>Block Storage for EC2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ebs/?p=tile</t>
+  </si>
+  <si>
+    <t>Amazon Elastic File System</t>
+  </si>
+  <si>
+    <t>Managed File Storage for EC2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/efs/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/glacier1/?p=tile</t>
+  </si>
+  <si>
+    <t>Amazon S3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/s3/?p=tile</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dms/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rds/aurora/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dynamodb/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>In-memory Data Store and Cache</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticache/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/neptune/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rds/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/redshift/?p=tile</t>
+  </si>
+  <si>
+    <t>Discover On-Premises Applications to Streamline Migration</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/application-discovery/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/migration-hub/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>Migrate On-Premises Servers to AWS</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/server-migration-service/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snowball/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/directconnect/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/api-gateway/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudfront/?p=tile</t>
+  </si>
+  <si>
+    <t>Scalable Domain Name System</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/route53/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/privatelink/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/vpc/?p=tile</t>
+  </si>
+  <si>
+    <t>Elastic Load Balancing</t>
+  </si>
+  <si>
+    <t>High Scale Load Balancing</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticloadbalancing/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloud9/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codebuild/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codecommit/?p=tile</t>
+  </si>
+  <si>
+    <t>Automate Code Deployment</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codedeploy/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codepipeline/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codestar/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cli/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/xray/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/autoscaling/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudformation/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudtrail/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/config/?p=tile</t>
+  </si>
+  <si>
+    <t>Automate Operations with Chef and Puppet</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/opsworks/?p=tile</t>
+  </si>
+  <si>
+    <t>Personalized View of AWS Service Health</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/premiumsupport/phd/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/servicecatalog/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/systems-manager/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/trustedadvisor/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudwatch/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediaconvert/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/medialive/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediapackage/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediastore/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediatailor/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elastictranscoder/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kinesis/video-streams/?p=tile</t>
+  </si>
+  <si>
+    <t>AWS Artifact</t>
+  </si>
+  <si>
+    <t>On-demand access to AWS compliance reports</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/artifact/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/certificate-manager/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudhsm/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/directoryservice/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/firewall-manager/?p=tile</t>
+  </si>
+  <si>
+    <t>AWS Identity &amp; Access Management</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iam/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kms/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/organizations/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/secrets-manager/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/shield/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/single-sign-on/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/waf/?p=tile</t>
+  </si>
+  <si>
+    <t>Create Flexible Cloud-native Directories</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloud-directory/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cognito/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/guardduty/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/inspector/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/macie/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>Orchestration Service for Periodic, Data-driven Workflows</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/datapipeline/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/glue/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/athena/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudsearch/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticmapreduce/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticsearch-service/?p=tile</t>
+  </si>
+  <si>
+    <t>Work with Real-time Streaming Data</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kinesis/?p=tile</t>
+  </si>
+  <si>
+    <t>Amazon Quicksight</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/quicksight/?p=tile</t>
+  </si>
+  <si>
+    <t>Quickly Start Deep Learning on EC2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/amazon-ai/amis/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/deeplens/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/comprehend/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lex/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/aml/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/polly/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rekognition/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sagemaker/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/transcribe/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/translate/?p=tile</t>
+  </si>
+  <si>
+    <t>Scalable, High-performance Deep Learning</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mxnet/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/tensorflow/?p=tile</t>
+  </si>
+  <si>
+    <t>Real-time and Offline Mobile Data Apps</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/appsync/?p=tile</t>
+  </si>
+  <si>
+    <t>Test Android, FireOS, and iOS Apps on Real Devices in the Cloud</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/device-farm/?p=tile</t>
+  </si>
+  <si>
+    <t>Build, Test, and Monitor Apps</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mobile/?p=tile</t>
+  </si>
+  <si>
+    <t>Mobile Software Development Kit</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mobile/sdk/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/pinpoint/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sumerian/?p=tile</t>
+  </si>
+  <si>
+    <t>Coordinate Distributed Applications</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/step-functions/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/amazon-mq/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sns/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sqs/?p=tile</t>
+  </si>
+  <si>
+    <t>Cloud-based Contact Center</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/connect/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ses/?p=tile</t>
+  </si>
+  <si>
+    <t>Empower your Organization with Alexa</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/alexaforbusiness/?p=tile</t>
+  </si>
+  <si>
+    <t>Frustration-free Meetings, Video Calls, and Chat</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/chime/?p=tile</t>
+  </si>
+  <si>
+    <t>Enterprise Storage and Sharing Service</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workdocs/?p=tile</t>
+  </si>
+  <si>
+    <t>Secure and Managed Business Email and Calendaring</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workmail/?p=tile</t>
+  </si>
+  <si>
+    <t>Stream Desktop Applications Securely to a Browser</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/appstream2/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>Desktop Computing Service</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workspaces/?hp=tile&amp;so-exp=below</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/greengrass/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-1-click/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-analytics/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot/button/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-core/?p=tile</t>
+  </si>
+  <si>
+    <t>Security Management for IoT devices</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-device-defender/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-device-management/?p=tile</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/freertos/?p=tile</t>
+  </si>
+  <si>
+    <t>Simple, Fast, Cost-effective Dedicated Game Server Hosting</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/gamelift/?p=tile</t>
+  </si>
+  <si>
+    <t>A Free Cross-Platform 3D Game Engine with Full Source, Integrated with AWS and Twitch</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lumberyard/?p=tile</t>
   </si>
 </sst>
 </file>
@@ -1460,8 +1406,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E143" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E143" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E135" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:E135" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="AWS Service" dataDxfId="2"/>
@@ -1738,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1765,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>423</v>
+        <v>235</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>228</v>
@@ -1782,11 +1728,11 @@
         <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E2" s="2" t="str">
-        <f t="shared" ref="D2:E33" si="0">HYPERLINK(D2,D2)</f>
-        <v>https://aws.amazon.com/batch/?nc2=h_l3_dm</v>
+        <f t="shared" ref="E2:E33" si="0">HYPERLINK(D2,D2)</f>
+        <v>https://aws.amazon.com/batch/?p=tile</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,11 +1746,11 @@
         <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/elasticbeanstalk/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/elasticbeanstalk/?p=tile</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1815,14 +1761,14 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/fargate/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/fargate/?p=tile</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1833,14 +1779,14 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/lambda/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/lambda/?p=tile</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1854,11 +1800,11 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/serverless/serverlessrepo/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/serverless/serverlessrepo/?p=tile</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1872,11 +1818,11 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/ec2/autoscaling/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/ec2/autoscaling/?p=tile</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1890,11 +1836,11 @@
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/ec2/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/ec2/?p=tile</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1908,11 +1854,11 @@
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/ecr/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/ecr/?p=tile</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1926,11 +1872,11 @@
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/eks/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/eks/?p=tile</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1944,11 +1890,11 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/ecs/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/ecs/?p=tile</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1962,11 +1908,11 @@
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>413</v>
+        <v>248</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/lightsail/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/lightsail/?p=tile</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1977,14 +1923,14 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/vmware/?nc2=h_l3_n</v>
+        <v>https://aws.amazon.com/vmware/?p=tile</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1998,11 +1944,11 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/snowball-edge/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/snowball-edge/?p=tile</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2016,11 +1962,11 @@
         <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/snowball/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/snowball/?p=tile</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2034,11 +1980,11 @@
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/snowmobile/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/snowmobile/?p=tile</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2052,11 +1998,11 @@
         <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/storagegateway/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/storagegateway/?p=tile</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2064,17 +2010,17 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>415</v>
+        <v>255</v>
       </c>
       <c r="C18" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/ebs/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/ebs/?p=tile</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2082,17 +2028,17 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="C19" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/efs/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/efs/?p=tile</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2106,11 +2052,11 @@
         <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/glacier/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/glacier1/?p=tile</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2118,22 +2064,22 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/s3/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/s3/?p=tile</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
@@ -2142,16 +2088,16 @@
         <v>49</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/dms/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/dms/?p=tile</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
@@ -2160,16 +2106,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/rds/aurora/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/rds/aurora/?p=tile</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
@@ -2178,34 +2124,34 @@
         <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/dynamodb/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/dynamodb/?hp=tile&amp;so-exp=below</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/elasticache/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/elasticache/?p=tile</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B26" t="s">
         <v>46</v>
@@ -2214,16 +2160,16 @@
         <v>47</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/neptune/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/neptune/?p=tile</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
@@ -2232,29 +2178,29 @@
         <v>40</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/rds/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/rds/?p=tile</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/redshift/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/redshift/?p=tile</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2265,14 +2211,14 @@
         <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/application-discovery/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/application-discovery/?p=tile</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2286,11 +2232,11 @@
         <v>49</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/dms/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/dms/?p=tile</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2304,11 +2250,11 @@
         <v>53</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/migration-hub/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/migration-hub/?hp=tile&amp;so-exp=below</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2319,14 +2265,14 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/server-migration-service/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/server-migration-service/?p=tile</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,11 +2286,11 @@
         <v>34</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="E33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/snowball-edge/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/snowball-edge/?p=tile</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2358,11 +2304,11 @@
         <v>32</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="E34" s="2" t="str">
-        <f t="shared" ref="D34:E65" si="1">HYPERLINK(D34,D34)</f>
-        <v>https://aws.amazon.com/snowball/?nc2=h_l3_sc</v>
+        <f t="shared" ref="E34:E65" si="1">HYPERLINK(D34,D34)</f>
+        <v>https://aws.amazon.com/snowball/?hp=tile&amp;so-exp=below</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2376,11 +2322,11 @@
         <v>36</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="E35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/snowmobile/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/snowmobile/?p=tile</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,11 +2340,11 @@
         <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/directconnect/?nc2=h_l3_n</v>
+        <v>https://aws.amazon.com/directconnect/?p=tile</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2412,11 +2358,11 @@
         <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/api-gateway/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/api-gateway/?p=tile</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2430,11 +2376,11 @@
         <v>59</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="E38" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/cloudfront/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/cloudfront/?p=tile</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2445,14 +2391,14 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="E39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/route53/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/route53/?p=tile</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,17 +2406,17 @@
         <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>416</v>
+        <v>233</v>
       </c>
       <c r="C40" t="s">
-        <v>417</v>
+        <v>234</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>418</v>
+        <v>284</v>
       </c>
       <c r="E40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/privatelink/?nc2=h_l3_n</v>
+        <v>https://aws.amazon.com/privatelink/?p=tile</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2484,29 +2430,29 @@
         <v>57</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="E41" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/vpc/?nc2=h_l3_n</v>
+        <v>https://aws.amazon.com/vpc/?p=tile</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>286</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>287</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="E42" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/cloud9/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/elasticloadbalancing/?p=tile</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2514,17 +2460,17 @@
         <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="E43" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/codebuild/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/cloud9/?p=tile</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2532,17 +2478,17 @@
         <v>65</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="E44" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/codecommit/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/codebuild/?p=tile</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2550,17 +2496,17 @@
         <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>279</v>
+        <v>69</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="E45" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/codedeploy/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/codecommit/?p=tile</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,17 +2514,17 @@
         <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>292</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="E46" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/codepipeline/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/codedeploy/?p=tile</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2586,17 +2532,17 @@
         <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="E47" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/codestar/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/codepipeline/?hp=tile&amp;so-exp=below</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2604,17 +2550,17 @@
         <v>65</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="E48" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/cli/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/codestar/?p=tile</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2622,17 +2568,17 @@
         <v>65</v>
       </c>
       <c r="B49" t="s">
-        <v>284</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>285</v>
+        <v>80</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>419</v>
+        <v>296</v>
       </c>
       <c r="E49" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/getting-started/tools-sdks/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/cli/?p=tile</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,11 +2592,11 @@
         <v>78</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="E50" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/xray/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/xray/?p=tile</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2664,11 +2610,11 @@
         <v>85</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="E51" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/autoscaling/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/autoscaling/?p=tile</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2682,11 +2628,11 @@
         <v>87</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="E52" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/cloudformation/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/cloudformation/?p=tile</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,11 +2646,11 @@
         <v>89</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="E53" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/cloudtrail/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/cloudtrail/?p=tile</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2712,17 +2658,17 @@
         <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="E54" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/cli/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/config/?p=tile</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2730,17 +2676,17 @@
         <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>302</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="E55" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/config/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/opsworks/?p=tile</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2748,17 +2694,17 @@
         <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>291</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="E56" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/managed-services/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/premiumsupport/phd/?p=tile</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2766,17 +2712,17 @@
         <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>294</v>
+        <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>295</v>
+        <v>94</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="E57" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/console/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/servicecatalog/?p=tile</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2784,17 +2730,17 @@
         <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C58" t="s">
-        <v>297</v>
+        <v>96</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="E58" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/opsworks/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/systems-manager/?p=tile</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2802,17 +2748,17 @@
         <v>81</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>299</v>
+        <v>98</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="E59" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/premiumsupport/phd/?nc2=h_l3_mt</v>
+        <v>https://aws.amazon.com/trustedadvisor/?p=tile</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2820,71 +2766,71 @@
         <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="E60" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/servicecatalog/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/cloudwatch/?p=tile</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C61" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="E61" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/systems-manager/?nc2=h_l3_mt</v>
+        <v>https://aws.amazon.com/mediaconvert/?p=tile</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="E62" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/premiumsupport/trustedadvisor/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/medialive/?p=tile</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="E63" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/cloudwatch/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/mediapackage/?p=tile</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2892,17 +2838,17 @@
         <v>100</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="E64" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/mediaconvert/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/mediastore/?p=tile</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2910,17 +2856,17 @@
         <v>100</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C65" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="E65" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://aws.amazon.com/medialive/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/mediatailor/?p=tile</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2928,17 +2874,17 @@
         <v>100</v>
       </c>
       <c r="B66" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C66" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="E66" s="2" t="str">
-        <f t="shared" ref="D66:E97" si="2">HYPERLINK(D66,D66)</f>
-        <v>https://aws.amazon.com/mediapackage/?nc2=h_l3_db</v>
+        <f t="shared" ref="E66:E97" si="2">HYPERLINK(D66,D66)</f>
+        <v>https://aws.amazon.com/elastictranscoder/?p=tile</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2946,71 +2892,71 @@
         <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="E67" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/mediastore/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/kinesis/video-streams/?p=tile</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B68" t="s">
-        <v>113</v>
+        <v>317</v>
       </c>
       <c r="C68" t="s">
-        <v>114</v>
+        <v>318</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="E68" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/mediatailor/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/artifact/?p=tile</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="E69" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/elastictranscoder/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/certificate-manager/?p=tile</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B70" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="C70" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="E70" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/kinesis/video-streams/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/cloudhsm/?p=tile</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,17 +2964,17 @@
         <v>115</v>
       </c>
       <c r="B71" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="E71" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/certificate-manager/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/directoryservice/?p=tile</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3036,17 +2982,17 @@
         <v>115</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>229</v>
       </c>
       <c r="C72" t="s">
-        <v>131</v>
+        <v>230</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="E72" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/cloudhsm/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/firewall-manager/?p=tile</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3054,17 +3000,17 @@
         <v>115</v>
       </c>
       <c r="B73" t="s">
-        <v>132</v>
+        <v>324</v>
       </c>
       <c r="C73" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="E73" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/directoryservice/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/iam/?p=tile</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3072,17 +3018,17 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>315</v>
+        <v>134</v>
       </c>
       <c r="C74" t="s">
-        <v>316</v>
+        <v>135</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="E74" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/firewall-manager/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/kms/?p=tile</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3090,17 +3036,17 @@
         <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>318</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="E75" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/iam/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/organizations/?p=tile</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3108,17 +3054,17 @@
         <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
       <c r="C76" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="E76" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/kms/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/secrets-manager/?p=tile</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3126,17 +3072,17 @@
         <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C77" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="E77" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/organizations/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/shield/?p=tile</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3144,17 +3090,17 @@
         <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>322</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>323</v>
+        <v>121</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="E78" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/secrets-manager/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/single-sign-on/?p=tile</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3162,17 +3108,17 @@
         <v>115</v>
       </c>
       <c r="B79" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C79" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="E79" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/shield/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/waf/?p=tile</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3180,17 +3126,17 @@
         <v>115</v>
       </c>
       <c r="B80" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C80" t="s">
-        <v>121</v>
+        <v>332</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="E80" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/single-sign-on/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/cloud-directory/?p=tile</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3198,17 +3144,17 @@
         <v>115</v>
       </c>
       <c r="B81" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="C81" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="E81" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/waf/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/cognito/?p=tile</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,17 +3162,17 @@
         <v>115</v>
       </c>
       <c r="B82" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C82" t="s">
-        <v>328</v>
+        <v>123</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="E82" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/cloud-directory/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/guardduty/?p=tile</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3234,17 +3180,17 @@
         <v>115</v>
       </c>
       <c r="B83" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="E83" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/cognito/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/inspector/?p=tile</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3252,179 +3198,179 @@
         <v>115</v>
       </c>
       <c r="B84" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C84" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="E84" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/guardduty/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/macie/?hp=tile&amp;so-exp=below</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="B85" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="C85" t="s">
-        <v>125</v>
+        <v>338</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="E85" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/inspector/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/datapipeline/?p=tile</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="C86" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="E86" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/macie/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/glue/?p=tile</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="C87" t="s">
-        <v>334</v>
+        <v>144</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>420</v>
+        <v>341</v>
       </c>
       <c r="E87" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/machine-learning/amis/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/athena/?p=tile</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="C88" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="E88" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/deeplens/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/cloudsearch/?p=tile</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B89" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C89" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="E89" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/comprehend/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/elasticmapreduce/?p=tile</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B90" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C90" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="E90" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/lex/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/elasticsearch-service/?p=tile</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B91" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C91" t="s">
-        <v>168</v>
+        <v>345</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="E91" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/aml/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/kinesis/?p=tile</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B92" t="s">
-        <v>163</v>
+        <v>347</v>
       </c>
       <c r="C92" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="E92" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/polly/?nc2=h_l3_c</v>
+        <v>https://aws.amazon.com/quicksight/?p=tile</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B93" t="s">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="C93" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>340</v>
+        <v>272</v>
       </c>
       <c r="E93" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/rekognition/?nc2=h_l3_sc</v>
+        <v>https://aws.amazon.com/redshift/?p=tile</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3432,17 +3378,17 @@
         <v>156</v>
       </c>
       <c r="B94" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="C94" t="s">
-        <v>158</v>
+        <v>349</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="E94" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/sagemaker/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/amazon-ai/amis/?p=tile</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3450,17 +3396,17 @@
         <v>156</v>
       </c>
       <c r="B95" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C95" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="E95" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/transcribe/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/deeplens/?p=tile</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3468,17 +3414,17 @@
         <v>156</v>
       </c>
       <c r="B96" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C96" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="E96" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/translate/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/comprehend/?p=tile</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3486,17 +3432,17 @@
         <v>156</v>
       </c>
       <c r="B97" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C97" t="s">
-        <v>344</v>
+        <v>162</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="E97" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>https://aws.amazon.com/mxnet/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/lex/?p=tile</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3504,179 +3450,179 @@
         <v>156</v>
       </c>
       <c r="B98" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="E98" s="2" t="str">
-        <f t="shared" ref="D98:E129" si="3">HYPERLINK(D98,D98)</f>
-        <v>https://aws.amazon.com/tensorflow/?nc2=h_l3_al</v>
+        <f t="shared" ref="E98:E129" si="3">HYPERLINK(D98,D98)</f>
+        <v>https://aws.amazon.com/aml/?p=tile</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B99" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C99" t="s">
-        <v>347</v>
+        <v>164</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="E99" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/datapipeline/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/polly/?p=tile</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B100" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C100" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="E100" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/glue/?nc2=h_l3_an</v>
+        <v>https://aws.amazon.com/rekognition/?p=tile</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B101" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="C101" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="E101" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/athena/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/sagemaker/?p=tile</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B102" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="C102" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="E102" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/cloudsearch/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/transcribe/?p=tile</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B103" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="C103" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E103" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/emr/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/translate/?p=tile</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B104" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="C104" t="s">
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="E104" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/elasticsearch-service/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/mxnet/?p=tile</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B105" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="C105" t="s">
-        <v>354</v>
+        <v>178</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="E105" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/kinesis/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/tensorflow/?p=tile</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="B106" t="s">
-        <v>356</v>
+        <v>183</v>
       </c>
       <c r="C106" t="s">
-        <v>152</v>
+        <v>363</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>414</v>
+        <v>364</v>
       </c>
       <c r="E106" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/quicksight/</v>
+        <v>https://aws.amazon.com/appsync/?p=tile</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="B107" t="s">
-        <v>44</v>
+        <v>184</v>
       </c>
       <c r="C107" t="s">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="E107" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/redshift/?nc2=h_l3_al</v>
+        <v>https://aws.amazon.com/device-farm/?p=tile</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3684,17 +3630,17 @@
         <v>179</v>
       </c>
       <c r="B108" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C108" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="E108" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/appsync/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/mobile/?p=tile</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3702,17 +3648,17 @@
         <v>179</v>
       </c>
       <c r="B109" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C109" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="E109" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/device-farm/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/mobile/sdk/?p=tile</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3720,17 +3666,17 @@
         <v>179</v>
       </c>
       <c r="B110" t="s">
-        <v>180</v>
+        <v>61</v>
       </c>
       <c r="C110" t="s">
-        <v>362</v>
+        <v>62</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>421</v>
+        <v>280</v>
       </c>
       <c r="E110" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/mobile/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/api-gateway/?p=tile</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3738,89 +3684,89 @@
         <v>179</v>
       </c>
       <c r="B111" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C111" t="s">
-        <v>363</v>
+        <v>182</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>422</v>
+        <v>371</v>
       </c>
       <c r="E111" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/mobile/resources/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/pinpoint/?p=tile</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B112" t="s">
-        <v>61</v>
+        <v>187</v>
       </c>
       <c r="C112" t="s">
-        <v>62</v>
+        <v>188</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>271</v>
+        <v>372</v>
       </c>
       <c r="E112" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/api-gateway/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/sumerian/?p=tile</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B113" t="s">
-        <v>118</v>
+        <v>190</v>
       </c>
       <c r="C113" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>330</v>
+        <v>374</v>
       </c>
       <c r="E113" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/cognito/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/step-functions/?p=tile</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B114" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="C114" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="E114" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/pinpoint/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/amazon-mq/?p=tile</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B115" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C115" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="E115" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/sumerian/?nc2=h_l3_db</v>
+        <v>https://aws.amazon.com/sns/?p=tile</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,251 +3774,251 @@
         <v>189</v>
       </c>
       <c r="B116" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C116" t="s">
-        <v>358</v>
+        <v>192</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="E116" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/appsync/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/sqs/?p=tile</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B117" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C117" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="E117" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/step-functions/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/connect/?p=tile</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B118" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="C118" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E118" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/amazon-mq/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/pinpoint/?p=tile</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B119" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C119" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="E119" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/sns/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/ses/?p=tile</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="B120" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="C120" t="s">
-        <v>192</v>
+        <v>381</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="E120" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/sqs/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/alexaforbusiness/?p=tile</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B121" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C121" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="E121" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/connect/?nc2=h_l3_cc</v>
+        <v>https://aws.amazon.com/chime/?p=tile</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B122" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="C122" t="s">
-        <v>182</v>
+        <v>385</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>365</v>
+        <v>386</v>
       </c>
       <c r="E122" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/pinpoint/?nc2=h_l3_ms</v>
+        <v>https://aws.amazon.com/workdocs/?p=tile</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B123" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C123" t="s">
-        <v>200</v>
+        <v>387</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="E123" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/ses/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/workmail/?p=tile</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B124" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C124" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="E124" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/alexaforbusiness/?nc2=h_l3_ap</v>
+        <v>https://aws.amazon.com/appstream2/?hp=tile&amp;so-exp=below</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B125" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C125" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="E125" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/chime/</v>
+        <v>https://aws.amazon.com/workspaces/?hp=tile&amp;so-exp=below</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B126" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="C126" t="s">
-        <v>379</v>
+        <v>215</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="E126" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/workdocs/?nc2=h_l3_ap</v>
+        <v>https://aws.amazon.com/greengrass/?p=tile</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B127" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="C127" t="s">
-        <v>381</v>
+        <v>217</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="E127" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/workmail/?nc2=h_l3_ap</v>
+        <v>https://aws.amazon.com/iot-1-click/?p=tile</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B128" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="C128" t="s">
-        <v>383</v>
+        <v>219</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="E128" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/appstream2/?nc2=h_l3_as</v>
+        <v>https://aws.amazon.com/iot-analytics/?p=tile</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B129" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="C129" t="s">
-        <v>385</v>
+        <v>221</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="E129" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>https://aws.amazon.com/workspaces/?nc2=h_l3_ap</v>
+        <v>https://aws.amazon.com/iot/button/?p=tile</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4080,17 +4026,17 @@
         <v>209</v>
       </c>
       <c r="B130" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C130" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="E130" s="2" t="str">
-        <f t="shared" ref="D130:E161" si="4">HYPERLINK(D130,D130)</f>
-        <v>https://aws.amazon.com/greengrass/?nc2=h_l3_ap</v>
+        <f t="shared" ref="E130:E135" si="4">HYPERLINK(D130,D130)</f>
+        <v>https://aws.amazon.com/iot-core/?p=tile</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4098,17 +4044,17 @@
         <v>209</v>
       </c>
       <c r="B131" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C131" t="s">
-        <v>217</v>
+        <v>398</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="E131" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/iot-1-click/?nc2=h_l3_ap</v>
+        <v>https://aws.amazon.com/iot-device-defender/?p=tile</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4116,17 +4062,17 @@
         <v>209</v>
       </c>
       <c r="B132" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C132" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="E132" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/iot-analytics/?nc2=h_l3_ap</v>
+        <v>https://aws.amazon.com/iot-device-management/?p=tile</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4134,197 +4080,53 @@
         <v>209</v>
       </c>
       <c r="B133" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C133" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="E133" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/iotbutton/</v>
+        <v>https://aws.amazon.com/freertos/?p=tile</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="B134" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="C134" t="s">
-        <v>211</v>
+        <v>402</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="E134" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/iot-core/?nc2=h_l3_ap</v>
+        <v>https://aws.amazon.com/gamelift/?p=tile</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="B135" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C135" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="E135" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/iot-device-defender/?nc2=h_l3_ap</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>209</v>
-      </c>
-      <c r="B136" t="s">
-        <v>223</v>
-      </c>
-      <c r="C136" t="s">
-        <v>224</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E136" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/iot-device-management/?nc2=h_l3_ap</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>209</v>
-      </c>
-      <c r="B137" t="s">
-        <v>212</v>
-      </c>
-      <c r="C137" t="s">
-        <v>213</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="E137" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/freertos/?nc2=h_l3_ap</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>225</v>
-      </c>
-      <c r="B138" t="s">
-        <v>226</v>
-      </c>
-      <c r="C138" t="s">
-        <v>396</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="E138" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/gamelift/?nc2=h_l3_ap</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>225</v>
-      </c>
-      <c r="B139" t="s">
-        <v>227</v>
-      </c>
-      <c r="C139" t="s">
-        <v>398</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E139" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/lumberyard/?nc2=h_l3_ap</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>400</v>
-      </c>
-      <c r="B140" t="s">
-        <v>401</v>
-      </c>
-      <c r="C140" t="s">
-        <v>402</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E140" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/aws-cost-management/aws-budgets/?nc2=h_l3_dm</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>400</v>
-      </c>
-      <c r="B141" t="s">
-        <v>404</v>
-      </c>
-      <c r="C141" t="s">
-        <v>405</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E141" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/aws-cost-management/aws-cost-explorer/?nc2=h_l3_dm</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>400</v>
-      </c>
-      <c r="B142" t="s">
-        <v>407</v>
-      </c>
-      <c r="C142" t="s">
-        <v>408</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="E142" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/aws-cost-management/aws-cost-and-usage-reporting/?nc2=h_l3_dm</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>400</v>
-      </c>
-      <c r="B143" t="s">
-        <v>410</v>
-      </c>
-      <c r="C143" t="s">
-        <v>411</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="E143" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>https://aws.amazon.com/aws-cost-management/reserved-instance-reporting/?nc2=h_l3_dm</v>
+        <v>https://aws.amazon.com/lumberyard/?p=tile</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename Service to Product
</commit_message>
<xml_diff>
--- a/AWS_Products.xlsx
+++ b/AWS_Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palsarma/git/github/palsarma/aws_products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3623B71E-F815-744E-9D7C-2BDB7EF25F2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7C5BD6-BCD4-B848-8B76-EDB15A98F2BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,9 +826,6 @@
     <t>Simple, Fast, Cost-effective Dedicated Game Server Hosting</t>
   </si>
   <si>
-    <t>Service</t>
-  </si>
-  <si>
     <t>https://aws.amazon.com/batch/?c=1&amp;pt=7</t>
   </si>
   <si>
@@ -1601,6 +1598,9 @@
   </si>
   <si>
     <t>https://aws.amazon.com/ground-station/?c=23&amp;pt=1</t>
+  </si>
+  <si>
+    <t>Product</t>
   </si>
 </sst>
 </file>
@@ -1684,20 +1684,6 @@
   <dxfs count="5">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1758,6 +1744,20 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -1772,13 +1772,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D171" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D171" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D171" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Service" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F37A6230-26FE-F443-B93E-E500764AE6AC}" name="Link" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Product" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F37A6230-26FE-F443-B93E-E500764AE6AC}" name="Link" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2052,8 +2052,8 @@
   </sheetPr>
   <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>264</v>
+        <v>522</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2090,7 +2090,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
         <v>225</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2132,7 +2132,7 @@
         <v>226</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2140,13 +2140,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" t="s">
         <v>269</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2160,7 +2160,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2174,7 +2174,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2216,7 +2216,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2258,7 +2258,7 @@
         <v>227</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2286,7 +2286,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2300,7 +2300,7 @@
         <v>35</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
         <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,7 +2328,7 @@
         <v>229</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>231</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2350,13 +2350,13 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" t="s">
         <v>286</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2364,13 +2364,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
+        <v>288</v>
+      </c>
+      <c r="C22" t="s">
         <v>289</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>25</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2412,7 +2412,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2451,10 +2451,10 @@
         <v>42</v>
       </c>
       <c r="C28" t="s">
+        <v>295</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2468,7 +2468,7 @@
         <v>46</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2476,13 +2476,13 @@
         <v>234</v>
       </c>
       <c r="B30" t="s">
+        <v>298</v>
+      </c>
+      <c r="C30" t="s">
         <v>299</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,7 +2496,7 @@
         <v>39</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,13 +2504,13 @@
         <v>234</v>
       </c>
       <c r="B32" t="s">
+        <v>302</v>
+      </c>
+      <c r="C32" t="s">
         <v>303</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2524,7 +2524,7 @@
         <v>44</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2532,18 +2532,18 @@
         <v>234</v>
       </c>
       <c r="B34" t="s">
+        <v>306</v>
+      </c>
+      <c r="C34" t="s">
         <v>307</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
@@ -2552,26 +2552,26 @@
         <v>235</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B36" t="s">
+        <v>311</v>
+      </c>
+      <c r="C36" t="s">
         <v>312</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B37" t="s">
         <v>47</v>
@@ -2580,12 +2580,12 @@
         <v>48</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B38" t="s">
         <v>50</v>
@@ -2594,12 +2594,12 @@
         <v>51</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B39" t="s">
         <v>52</v>
@@ -2608,12 +2608,12 @@
         <v>236</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B40" t="s">
         <v>30</v>
@@ -2622,12 +2622,12 @@
         <v>31</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
@@ -2636,12 +2636,12 @@
         <v>33</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B42" t="s">
         <v>34</v>
@@ -2650,21 +2650,21 @@
         <v>35</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B43" t="s">
+        <v>320</v>
+      </c>
+      <c r="C43" t="s">
         <v>321</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2672,13 +2672,13 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
+        <v>323</v>
+      </c>
+      <c r="C44" t="s">
         <v>324</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,13 +2686,13 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
+        <v>326</v>
+      </c>
+      <c r="C45" t="s">
         <v>327</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2706,7 +2706,7 @@
         <v>62</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2714,13 +2714,13 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
+        <v>330</v>
+      </c>
+      <c r="C47" t="s">
         <v>331</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,13 +2728,13 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
+        <v>333</v>
+      </c>
+      <c r="C48" t="s">
         <v>334</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2748,7 +2748,7 @@
         <v>60</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2762,7 +2762,7 @@
         <v>57</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2776,7 +2776,7 @@
         <v>237</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
         <v>55</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2801,10 +2801,10 @@
         <v>224</v>
       </c>
       <c r="C53" t="s">
+        <v>340</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2818,7 +2818,7 @@
         <v>239</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2832,7 +2832,7 @@
         <v>74</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>69</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
         <v>67</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2874,7 +2874,7 @@
         <v>240</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2888,7 +2888,7 @@
         <v>72</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
         <v>65</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2916,7 +2916,7 @@
         <v>78</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2930,12 +2930,12 @@
         <v>76</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B63" t="s">
         <v>81</v>
@@ -2944,12 +2944,12 @@
         <v>82</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B64" t="s">
         <v>83</v>
@@ -2958,12 +2958,12 @@
         <v>84</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B65" t="s">
         <v>85</v>
@@ -2972,12 +2972,12 @@
         <v>86</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B66" t="s">
         <v>87</v>
@@ -2986,40 +2986,40 @@
         <v>88</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B67" t="s">
+        <v>356</v>
+      </c>
+      <c r="C67" t="s">
         <v>357</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B68" t="s">
+        <v>359</v>
+      </c>
+      <c r="C68" t="s">
         <v>360</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B69" t="s">
         <v>89</v>
@@ -3028,12 +3028,12 @@
         <v>241</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B70" t="s">
         <v>96</v>
@@ -3042,12 +3042,12 @@
         <v>242</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B71" t="s">
         <v>90</v>
@@ -3056,12 +3056,12 @@
         <v>91</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B72" t="s">
         <v>92</v>
@@ -3070,12 +3070,12 @@
         <v>93</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B73" t="s">
         <v>94</v>
@@ -3084,26 +3084,26 @@
         <v>95</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B74" t="s">
+        <v>367</v>
+      </c>
+      <c r="C74" t="s">
         <v>368</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B75" t="s">
         <v>79</v>
@@ -3112,7 +3112,7 @@
         <v>80</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3120,13 +3120,13 @@
         <v>97</v>
       </c>
       <c r="B76" t="s">
+        <v>371</v>
+      </c>
+      <c r="C76" t="s">
         <v>372</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>103</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
         <v>105</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3168,7 +3168,7 @@
         <v>107</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3182,7 +3182,7 @@
         <v>109</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3196,7 +3196,7 @@
         <v>111</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3210,7 +3210,7 @@
         <v>99</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>101</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3238,7 +3238,7 @@
         <v>244</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3252,7 +3252,7 @@
         <v>125</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,7 +3266,7 @@
         <v>127</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3280,7 +3280,7 @@
         <v>129</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3294,7 +3294,7 @@
         <v>221</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3308,7 +3308,7 @@
         <v>113</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3322,7 +3322,7 @@
         <v>131</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3336,7 +3336,7 @@
         <v>133</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -3350,7 +3350,7 @@
         <v>223</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3358,13 +3358,13 @@
         <v>112</v>
       </c>
       <c r="B93" t="s">
+        <v>390</v>
+      </c>
+      <c r="C93" t="s">
         <v>391</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3378,7 +3378,7 @@
         <v>135</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>118</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
         <v>137</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3420,7 +3420,7 @@
         <v>246</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3434,7 +3434,7 @@
         <v>116</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3448,7 +3448,7 @@
         <v>120</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
         <v>122</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3473,10 +3473,10 @@
         <v>123</v>
       </c>
       <c r="C101" t="s">
+        <v>400</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3490,7 +3490,7 @@
         <v>247</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,7 +3504,7 @@
         <v>151</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,13 +3512,13 @@
         <v>138</v>
       </c>
       <c r="B104" t="s">
+        <v>404</v>
+      </c>
+      <c r="C104" t="s">
         <v>405</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3532,7 +3532,7 @@
         <v>140</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
         <v>144</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3560,7 +3560,7 @@
         <v>142</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,7 +3574,7 @@
         <v>146</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3588,7 +3588,7 @@
         <v>248</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,13 +3596,13 @@
         <v>138</v>
       </c>
       <c r="B110" t="s">
+        <v>412</v>
+      </c>
+      <c r="C110" t="s">
         <v>413</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3616,7 +3616,7 @@
         <v>148</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,7 +3630,7 @@
         <v>44</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3644,7 +3644,7 @@
         <v>250</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,7 +3658,7 @@
         <v>168</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3666,13 +3666,13 @@
         <v>152</v>
       </c>
       <c r="B115" t="s">
+        <v>419</v>
+      </c>
+      <c r="C115" t="s">
         <v>420</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3686,7 +3686,7 @@
         <v>156</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3694,13 +3694,13 @@
         <v>152</v>
       </c>
       <c r="B117" t="s">
+        <v>423</v>
+      </c>
+      <c r="C117" t="s">
         <v>424</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3708,13 +3708,13 @@
         <v>152</v>
       </c>
       <c r="B118" t="s">
+        <v>426</v>
+      </c>
+      <c r="C118" t="s">
         <v>427</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,13 +3722,13 @@
         <v>152</v>
       </c>
       <c r="B119" t="s">
+        <v>429</v>
+      </c>
+      <c r="C119" t="s">
         <v>430</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3742,7 +3742,7 @@
         <v>158</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,13 +3750,13 @@
         <v>152</v>
       </c>
       <c r="B121" t="s">
+        <v>433</v>
+      </c>
+      <c r="C121" t="s">
         <v>434</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3770,7 +3770,7 @@
         <v>160</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3784,7 +3784,7 @@
         <v>162</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,7 +3798,7 @@
         <v>154</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3806,13 +3806,13 @@
         <v>152</v>
       </c>
       <c r="B125" t="s">
+        <v>439</v>
+      </c>
+      <c r="C125" t="s">
         <v>440</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D125" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3820,13 +3820,13 @@
         <v>152</v>
       </c>
       <c r="B126" t="s">
+        <v>442</v>
+      </c>
+      <c r="C126" t="s">
         <v>443</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3840,7 +3840,7 @@
         <v>166</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3854,7 +3854,7 @@
         <v>164</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3868,7 +3868,7 @@
         <v>251</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3882,26 +3882,26 @@
         <v>172</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>449</v>
+      </c>
+      <c r="B131" t="s">
         <v>450</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>451</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B132" t="s">
         <v>175</v>
@@ -3910,12 +3910,12 @@
         <v>252</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B133" t="s">
         <v>176</v>
@@ -3924,12 +3924,12 @@
         <v>253</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B134" t="s">
         <v>177</v>
@@ -3938,12 +3938,12 @@
         <v>254</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B135" t="s">
         <v>59</v>
@@ -3952,12 +3952,12 @@
         <v>60</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B136" t="s">
         <v>173</v>
@@ -3966,7 +3966,7 @@
         <v>174</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3980,7 +3980,7 @@
         <v>180</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3994,7 +3994,7 @@
         <v>255</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -4008,7 +4008,7 @@
         <v>188</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -4022,7 +4022,7 @@
         <v>186</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
         <v>184</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4050,7 +4050,7 @@
         <v>256</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4064,7 +4064,7 @@
         <v>174</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4078,12 +4078,12 @@
         <v>192</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B145" t="s">
         <v>193</v>
@@ -4092,12 +4092,12 @@
         <v>257</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B146" t="s">
         <v>194</v>
@@ -4106,12 +4106,12 @@
         <v>258</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B147" t="s">
         <v>195</v>
@@ -4120,12 +4120,12 @@
         <v>259</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B148" t="s">
         <v>196</v>
@@ -4134,7 +4134,7 @@
         <v>260</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4148,7 +4148,7 @@
         <v>261</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4162,7 +4162,7 @@
         <v>262</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>206</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4190,7 +4190,7 @@
         <v>208</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4204,7 +4204,7 @@
         <v>210</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,7 +4218,7 @@
         <v>212</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,7 +4232,7 @@
         <v>202</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4243,10 +4243,10 @@
         <v>213</v>
       </c>
       <c r="C156" t="s">
+        <v>478</v>
+      </c>
+      <c r="D156" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4260,7 +4260,7 @@
         <v>215</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4268,13 +4268,13 @@
         <v>200</v>
       </c>
       <c r="B158" t="s">
+        <v>481</v>
+      </c>
+      <c r="C158" t="s">
         <v>482</v>
       </c>
-      <c r="C158" t="s">
+      <c r="D158" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4282,13 +4282,13 @@
         <v>200</v>
       </c>
       <c r="B159" t="s">
+        <v>484</v>
+      </c>
+      <c r="C159" t="s">
         <v>485</v>
       </c>
-      <c r="C159" t="s">
+      <c r="D159" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,13 +4296,13 @@
         <v>200</v>
       </c>
       <c r="B160" t="s">
+        <v>487</v>
+      </c>
+      <c r="C160" t="s">
         <v>488</v>
       </c>
-      <c r="C160" t="s">
+      <c r="D160" s="2" t="s">
         <v>489</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4310,13 +4310,13 @@
         <v>200</v>
       </c>
       <c r="B161" t="s">
+        <v>490</v>
+      </c>
+      <c r="C161" t="s">
         <v>491</v>
       </c>
-      <c r="C161" t="s">
+      <c r="D161" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4330,7 +4330,7 @@
         <v>204</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4344,7 +4344,7 @@
         <v>263</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4355,108 +4355,108 @@
         <v>218</v>
       </c>
       <c r="C164" t="s">
+        <v>495</v>
+      </c>
+      <c r="D164" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>497</v>
+      </c>
+      <c r="B165" t="s">
         <v>498</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
         <v>499</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D165" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="D165" s="2" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B166" t="s">
+        <v>501</v>
+      </c>
+      <c r="C166" t="s">
         <v>502</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D166" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B167" t="s">
+        <v>504</v>
+      </c>
+      <c r="C167" t="s">
         <v>505</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D167" s="2" t="s">
         <v>506</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B168" t="s">
+        <v>507</v>
+      </c>
+      <c r="C168" t="s">
         <v>508</v>
       </c>
-      <c r="C168" t="s">
+      <c r="D168" s="2" t="s">
         <v>509</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>510</v>
+      </c>
+      <c r="B169" t="s">
         <v>511</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>512</v>
       </c>
-      <c r="C169" t="s">
+      <c r="D169" s="2" t="s">
         <v>513</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>514</v>
+      </c>
+      <c r="B170" t="s">
         <v>515</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>516</v>
       </c>
-      <c r="C170" t="s">
+      <c r="D170" s="2" t="s">
         <v>517</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>518</v>
+      </c>
+      <c r="B171" t="s">
         <v>519</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" t="s">
         <v>520</v>
       </c>
-      <c r="C171" t="s">
+      <c r="D171" s="2" t="s">
         <v>521</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to output files
</commit_message>
<xml_diff>
--- a/AWS_Products.xlsx
+++ b/AWS_Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palsarma/git/github/palsarma/aws_products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7C5BD6-BCD4-B848-8B76-EDB15A98F2BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B340D-2551-5D44-8D31-871BC1CA56A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="534">
   <si>
     <t>Category</t>
   </si>
@@ -124,24 +124,6 @@
     <t>Hybrid Storage Integration</t>
   </si>
   <si>
-    <t>AWS Snowball</t>
-  </si>
-  <si>
-    <t>Petabyte-scale Data Transport</t>
-  </si>
-  <si>
-    <t>AWS Snowball Edge</t>
-  </si>
-  <si>
-    <t>Petabyte-scale Data Transport with On-board Compute</t>
-  </si>
-  <si>
-    <t>AWS Snowmobile</t>
-  </si>
-  <si>
-    <t>Exabyte-scale Data Transport</t>
-  </si>
-  <si>
     <t>Amazon Aurora</t>
   </si>
   <si>
@@ -565,9 +547,6 @@
     <t>AWS Device Farm</t>
   </si>
   <si>
-    <t>AWS Mobile SDK</t>
-  </si>
-  <si>
     <t>AR &amp; VR</t>
   </si>
   <si>
@@ -682,9 +661,6 @@
     <t>Onboard, Organize, and Remotely Manage IoT Devices</t>
   </si>
   <si>
-    <t>Game Development</t>
-  </si>
-  <si>
     <t>Amazon GameLift</t>
   </si>
   <si>
@@ -718,24 +694,6 @@
     <t>Build a Hybrid Cloud without Custom Hardware</t>
   </si>
   <si>
-    <t>Amazon EBS</t>
-  </si>
-  <si>
-    <t>Block Storage for EC2</t>
-  </si>
-  <si>
-    <t>Amazon Elastic File System</t>
-  </si>
-  <si>
-    <t>Managed File Storage for EC2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/glacier1/?p=tile</t>
-  </si>
-  <si>
-    <t>Amazon S3</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -751,9 +709,6 @@
     <t>Elastic Load Balancing</t>
   </si>
   <si>
-    <t>High Scale Load Balancing</t>
-  </si>
-  <si>
     <t>Automate Code Deployment</t>
   </si>
   <si>
@@ -796,9 +751,6 @@
     <t>Test Android, FireOS, and iOS Apps on Real Devices in the Cloud</t>
   </si>
   <si>
-    <t>Mobile Software Development Kit</t>
-  </si>
-  <si>
     <t>Coordinate Distributed Applications</t>
   </si>
   <si>
@@ -826,561 +778,177 @@
     <t>Simple, Fast, Cost-effective Dedicated Game Server Hosting</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/batch/?c=1&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elasticbeanstalk/?c=1&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/fargate/?c=1&amp;pt=9</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/lambda/?c=1&amp;pt=10</t>
-  </si>
-  <si>
     <t>AWS Outposts</t>
   </si>
   <si>
     <t>Run AWS services on-premises</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/outposts/?c=1&amp;pt=13</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/serverlessrepo/?c=1&amp;pt=11</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/?c=1&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/autoscaling/?c=1&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ecr/?c=1&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ecs/?c=1&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/eks/?c=1&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/lightsail/?c=1&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/vmware/?c=1&amp;pt=12</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowball/?c=2&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowball-edge/?c=2&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowmobile/?c=2&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/storagegateway/?c=2&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ebs/?c=2&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/efs/?c=2&amp;pt=3</t>
-  </si>
-  <si>
     <t>Amazon FSx for Lustre</t>
   </si>
   <si>
     <t>Fully managed compute-intensive file system</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/fsx/lustre/?c=2&amp;pt=8</t>
-  </si>
-  <si>
     <t>Amazon FSx for Windows File Server</t>
   </si>
   <si>
     <t>Fully managed Windows native file system</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/fsx/windows/?c=2&amp;pt=9</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/s3/?c=2&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/dms/?c=3&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/rds/aurora/?c=3&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/dynamodb/?c=3&amp;pt=3</t>
-  </si>
-  <si>
     <t>In-memory Caching System</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/elasticache/?c=3&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/neptune/?c=3&amp;pt=6</t>
-  </si>
-  <si>
     <t>Amazon Quantum Ledger Database (QLDB)</t>
   </si>
   <si>
     <t>Fully managed ledger database</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/qldb/?c=3&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/rds/?c=3&amp;pt=2</t>
-  </si>
-  <si>
     <t>Amazon RDS on VMware</t>
   </si>
   <si>
     <t>Automate on-premises database management</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/rds/vmware/?c=3&amp;pt=10</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/redshift/?c=3&amp;pt=5</t>
-  </si>
-  <si>
     <t>Amazon Timestream</t>
   </si>
   <si>
     <t>Fully managed time series database</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/timestream/?c=3&amp;pt=9</t>
-  </si>
-  <si>
     <t>Migration &amp; Transfer</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/application-discovery/?c=4&amp;pt=1</t>
-  </si>
-  <si>
     <t>AWS DataSync</t>
   </si>
   <si>
     <t>Simple, fast, online data transfer</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/datasync/?c=4&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/dms/?c=4&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/migration-hub/?c=4&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/server-migration-service/?c=4&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowball/?c=4&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowball-edge/?c=4&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/snowmobile/?c=4&amp;pt=7</t>
-  </si>
-  <si>
     <t>AWS Transfer for SFTP</t>
   </si>
   <si>
     <t>Fully managed SFTP service</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/sftp/?c=4&amp;pt=9</t>
-  </si>
-  <si>
     <t>AWS App Mesh</t>
   </si>
   <si>
     <t>Monitor and control microservices</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/app-mesh/?c=5&amp;pt=9</t>
-  </si>
-  <si>
     <t>AWS Cloud Map</t>
   </si>
   <si>
     <t>Application resource registry for microservices</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/cloud-map/?c=5&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/directconnect/?c=5&amp;pt=6</t>
-  </si>
-  <si>
     <t>AWS Global Accelerator</t>
   </si>
   <si>
     <t>Improve application availability and performance</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/global-accelerator/?c=5&amp;pt=11</t>
-  </si>
-  <si>
     <t>AWS Transit Gateway</t>
   </si>
   <si>
     <t>Easily scale VPC and account connections</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/transit-gateway/?c=5&amp;pt=10</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/api-gateway/?c=5&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudfront/?c=5&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/route53/?c=5&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/vpc/?c=5&amp;pt=1</t>
-  </si>
-  <si>
     <t>Securely Access Services Hosted on AWS</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/privatelink/?c=5&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elasticloadbalancing/?c=5&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloud9/?c=6&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codebuild/?c=6&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codecommit/?c=6&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codedeploy/?c=6&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codepipeline/?c=6&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/codestar/?c=6&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cli/?c=6&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/xray/?c=6&amp;pt=7</t>
-  </si>
-  <si>
     <t>Management &amp; Governance</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/autoscaling/?c=7&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudformation/?c=7&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudtrail/?c=7&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/config/?c=7&amp;pt=5</t>
-  </si>
-  <si>
     <t>AWS Control Tower</t>
   </si>
   <si>
     <t>Set up and govern a secure, compliant, multi-account environment</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/controltower/?c=7&amp;pt=11</t>
-  </si>
-  <si>
     <t>AWS License Manager</t>
   </si>
   <si>
     <t>Track, manage, and control licenses</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/license-manager/?c=7&amp;pt=12</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/opsworks/?c=7&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/premiumsupport/phd/?c=7&amp;pt=10</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/servicecatalog/?c=7&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/systems-manager/?c=7&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/trustedadvisor/?c=7&amp;pt=9</t>
-  </si>
-  <si>
     <t>AWS Well-Architected Tool</t>
   </si>
   <si>
     <t>Review and improve your workloads</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/well-architected-tool/?c=7&amp;pt=13</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudwatch/?c=7&amp;pt=1</t>
-  </si>
-  <si>
     <t>AWS Elemental MediaConnect</t>
   </si>
   <si>
     <t>Reliable and secure live video transport</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/mediaconnect/?c=8&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediaconvert/?c=8&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/medialive/?c=8&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediapackage/?c=8&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediastore/?c=8&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mediatailor/?c=8&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elastictranscoder/?c=8&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/kinesis/video-streams/?c=8&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/artifact/?c=9&amp;pt=17</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/certificate-manager/?c=9&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudhsm/?c=9&amp;pt=9</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/directoryservice/?c=9&amp;pt=10</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/firewall-manager/?c=9&amp;pt=11</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iam/?c=9&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/kms/?c=9&amp;pt=12</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/organizations/?c=9&amp;pt=13</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/secrets-manager/?c=9&amp;pt=14</t>
-  </si>
-  <si>
     <t>AWS Security Hub</t>
   </si>
   <si>
     <t>Unified security and compliance center</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/security-hub/?c=9&amp;pt=18</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/shield/?c=9&amp;pt=15</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/single-sign-on/?c=9&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/waf/?c=9&amp;pt=16</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloud-directory/?c=9&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cognito/?c=9&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/guardduty/?c=9&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/inspector/?c=9&amp;pt=6</t>
-  </si>
-  <si>
     <t>Discover, Classify, and Protect your Data</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/macie/?c=9&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/datapipeline/?c=10&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/glue/?c=10&amp;pt=9</t>
-  </si>
-  <si>
     <t>AWS Lake Formation</t>
   </si>
   <si>
     <t>Build a secure data lake in days</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/lake-formation/?c=10&amp;pt=11</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/athena/?c=10&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudsearch/?c=10&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elasticmapreduce/?c=10&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/elasticsearch-service/?c=10&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/kinesis/?c=10&amp;pt=5</t>
-  </si>
-  <si>
     <t>Amazon Managed Streaming for Kafka</t>
   </si>
   <si>
     <t>Fully managed Apache Kafka service</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/msk/?c=10&amp;pt=10</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/quicksight/?c=10&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/redshift/?c=10&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/machine-learning/amis/?c=11&amp;pt=10</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/deeplens/?c=11&amp;pt=9</t>
-  </si>
-  <si>
     <t>AWS DeepRacer</t>
   </si>
   <si>
     <t>Autonomous 1/18th scale race car, driven by ML</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/deepracer/?c=11&amp;pt=19</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/comprehend/?c=11&amp;pt=2</t>
-  </si>
-  <si>
     <t>Amazon Elastic Inference</t>
   </si>
   <si>
     <t>Deep learning inference acceleration</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/elastic-inference/?c=11&amp;pt=17</t>
-  </si>
-  <si>
     <t>Amazon Forecast</t>
   </si>
   <si>
     <t>Increase forecast accuracy using machine learning</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/forecast/?c=11&amp;pt=14</t>
-  </si>
-  <si>
     <t>Amazon Inferentia</t>
   </si>
   <si>
     <t>Machine learning inference chip</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/inferentia/?c=11&amp;pt=15</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/lex/?c=11&amp;pt=3</t>
-  </si>
-  <si>
     <t>Amazon Personalize</t>
   </si>
   <si>
     <t>Build real-time recommendations into your applications</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/personalize/?c=11&amp;pt=13</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/polly/?c=11&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/rekognition/?c=11&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sagemaker/?c=11&amp;pt=1</t>
-  </si>
-  <si>
     <t>Amazon SageMaker Ground Truth</t>
   </si>
   <si>
     <t>Build accurate ML training datasets</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/sagemaker/groundtruth/?c=11&amp;pt=18</t>
-  </si>
-  <si>
     <t>Amazon Textract</t>
   </si>
   <si>
     <t>Extract text and data from documents</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/textract/?c=11&amp;pt=16</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/transcribe/?c=11&amp;pt=8</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/translate/?c=11&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mxnet/?c=11&amp;pt=11</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/tensorflow/?c=11&amp;pt=12</t>
-  </si>
-  <si>
     <t>Mobile</t>
   </si>
   <si>
@@ -1390,141 +958,39 @@
     <t>Build and deploy mobile and web applications</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/amplify/?c=12&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/appsync/?c=12&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/device-farm/?c=12&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/mobile/sdk/?c=12&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/api-gateway/?c=12&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/pinpoint/?c=12&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sumerian/?c=13&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/step-functions/?c=14&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/amazon-mq/?c=14&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sns/?c=14&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/sqs/?c=14&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/connect/?c=15&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/pinpoint/?c=15&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ses/?c=15&amp;pt=3</t>
-  </si>
-  <si>
     <t>Business Applications</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/alexaforbusiness/?c=16&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/chime/?c=16&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/workdocs/?c=16&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/workmail/?c=16&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/appstream2/?c=17&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/workspaces/?c=17&amp;pt=1</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/greengrass/?c=18&amp;pt=3</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-1-click/?c=18&amp;pt=4</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-analytics/?c=18&amp;pt=5</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot/button/?c=18&amp;pt=6</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-core/?c=18&amp;pt=1</t>
-  </si>
-  <si>
     <t>Security Management for IoT Devices</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/iot-device-defender/?c=18&amp;pt=7</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/iot-device-management/?c=18&amp;pt=8</t>
-  </si>
-  <si>
     <t>AWS IoT Events</t>
   </si>
   <si>
     <t>IoT event detection and response</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/iot-events/?c=18&amp;pt=9</t>
-  </si>
-  <si>
     <t>AWS IoT SiteWise</t>
   </si>
   <si>
     <t>IoT data collector and interpreter</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/iot-sitewise/?c=18&amp;pt=10</t>
-  </si>
-  <si>
     <t>AWS IoT Things Graph</t>
   </si>
   <si>
     <t>Easily connect devices and web services</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/iot-things-graph/?c=18&amp;pt=12</t>
-  </si>
-  <si>
     <t>AWS Partner Device Catalog</t>
   </si>
   <si>
     <t>Curated catalog of AWS-compatible IoT hardware</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/partners/dqp/?c=18&amp;pt=11</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/freertos/?c=18&amp;pt=2</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/gamelift/?c=19&amp;pt=1</t>
-  </si>
-  <si>
     <t>A Free Cross-platform 3D Game Engine with Full Source, Integrated with AWS and Twitch</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/lumberyard/?c=19&amp;pt=2</t>
-  </si>
-  <si>
     <t>AWS Cost Management</t>
   </si>
   <si>
@@ -1534,36 +1000,24 @@
     <t>Set Custom Cost and Usage Budgets</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/aws-cost-management/aws-budgets/?c=20&amp;pt=2</t>
-  </si>
-  <si>
     <t>AWS Cost Explorer</t>
   </si>
   <si>
     <t>Analyze Your AWS Cost and Usage</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/aws-cost-management/aws-cost-explorer/?c=20&amp;pt=1</t>
-  </si>
-  <si>
     <t>AWS Cost and Usage Report</t>
   </si>
   <si>
     <t>Access Comprehensive Cost and Usage Information</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/aws-cost-management/aws-cost-and-usage-reporting/?c=20&amp;pt=4</t>
-  </si>
-  <si>
     <t>Reserved Instance Reporting</t>
   </si>
   <si>
     <t>Dive Deeper into Your Reserved Instances (RIs)</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/aws-cost-management/reserved-instance-reporting/?c=20&amp;pt=3</t>
-  </si>
-  <si>
     <t>Blockchain</t>
   </si>
   <si>
@@ -1573,9 +1027,6 @@
     <t>Create and manage scalable blockchain networks</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/blockchain/?c=21&amp;pt=1</t>
-  </si>
-  <si>
     <t>Robotics</t>
   </si>
   <si>
@@ -1585,9 +1036,6 @@
     <t>Develop, test, and deploy robotics applications</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/robomaker/?c=22&amp;pt=1</t>
-  </si>
-  <si>
     <t>Satellite</t>
   </si>
   <si>
@@ -1597,10 +1045,595 @@
     <t>Fully managed ground station as a service</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/ground-station/?c=23&amp;pt=1</t>
-  </si>
-  <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/datapipeline/?c=1&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/glue/?c=1&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lake-formation/?c=1&amp;pt=11</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/athena/?c=1&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudsearch/?c=1&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticmapreduce/?c=1&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticsearch-service/?c=1&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kinesis/?c=1&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/msk/?c=1&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/quicksight/?c=1&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/redshift/?c=1&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/step-functions/?c=2&amp;pt=1</t>
+  </si>
+  <si>
+    <t>Amazon AppSync</t>
+  </si>
+  <si>
+    <t>Build data-driven apps with real-time and offline capabilities</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/appsync/?c=2&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/amazon-mq/?c=2&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sns/?c=2&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sqs/?c=2&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sumerian/?c=3&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/aws-cost-management/aws-budgets/?c=4&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/aws-cost-management/aws-cost-explorer/?c=4&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/aws-cost-management/aws-cost-and-usage-reporting/?c=4&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/aws-cost-management/reserved-instance-reporting/?c=4&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/blockchain/?c=5&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/qldb/?c=5&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/alexaforbusiness/?c=6&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/chime/?c=6&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workdocs/?c=6&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workmail/?c=6&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/batch/?c=7&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticbeanstalk/?c=7&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/fargate/?c=7&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lambda/?c=7&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/outposts/?c=7&amp;pt=13</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/serverlessrepo/?c=7&amp;pt=11</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/?c=7&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/autoscaling/?c=7&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ecr/?c=7&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ecs/?c=7&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/eks/?c=7&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lightsail/?c=7&amp;pt=6</t>
+  </si>
+  <si>
+    <t>Distribute incoming traffic across multiple targets</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticloadbalancing/?c=7&amp;pt=14</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/vmware/?c=7&amp;pt=12</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/connect/?c=8&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/pinpoint/?c=8&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ses/?c=8&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dms/?c=9&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rds/aurora/?c=9&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dynamodb/?c=9&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elasticache/?c=9&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/neptune/?c=9&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/qldb/?c=9&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rds/?c=9&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rds/vmware/?c=9&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/redshift/?c=9&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/timestream/?c=9&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/appstream2/?c=10&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/workspaces/?c=10&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloud9/?c=11&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codebuild/?c=11&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codecommit/?c=11&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codedeploy/?c=11&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codepipeline/?c=11&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codestar/?c=11&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cli/?c=11&amp;pt=8</t>
+  </si>
+  <si>
+    <t>AWS Tools and SDKs</t>
+  </si>
+  <si>
+    <t>Tools and SDKs for AWS</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/getting-started/tools-sdks/?c=11&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/xray/?c=11&amp;pt=7</t>
+  </si>
+  <si>
+    <t>Amazon Corretto</t>
+  </si>
+  <si>
+    <t>Production-ready distribution of OpenJDK</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/corretto/?c=11&amp;pt=9</t>
+  </si>
+  <si>
+    <t>Game Tech</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/gamelift/?c=12&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lumberyard/?c=12&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/greengrass/?c=13&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-1-click/?c=13&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-analytics/?c=13&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot/button/?c=13&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-core/?c=13&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-device-defender/?c=13&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-device-management/?c=13&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-events/?c=13&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-sitewise/?c=13&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iot-things-graph/?c=13&amp;pt=12</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/partners/dqp/?c=13&amp;pt=11</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/freertos/?c=13&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/machine-learning/amis/?c=14&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/deeplens/?c=14&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/deepracer/?c=14&amp;pt=19</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/comprehend/?c=14&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elastic-inference/?c=14&amp;pt=17</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/forecast/?c=14&amp;pt=14</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/inferentia/?c=14&amp;pt=15</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lex/?c=14&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/personalize/?c=14&amp;pt=13</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/polly/?c=14&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/rekognition/?c=14&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sagemaker/?c=14&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sagemaker/groundtruth/?c=14&amp;pt=18</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/textract/?c=14&amp;pt=16</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/transcribe/?c=14&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/translate/?c=14&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mxnet/?c=14&amp;pt=11</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/tensorflow/?c=14&amp;pt=12</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/autoscaling/?c=15&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudformation/?c=15&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudtrail/?c=15&amp;pt=4</t>
+  </si>
+  <si>
+    <t>Unified tool to manage AWS services</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cli/?c=15&amp;pt=14</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/config/?c=15&amp;pt=5</t>
+  </si>
+  <si>
+    <t>AWS Console Mobile Application</t>
+  </si>
+  <si>
+    <t>Access resources on the go</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/console/mobile/?c=15&amp;pt=15</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/controltower/?c=15&amp;pt=11</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/license-manager/?c=15&amp;pt=12</t>
+  </si>
+  <si>
+    <t>AWS Managed Services</t>
+  </si>
+  <si>
+    <t>Infrastructure operations management for AWS</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/managed-services/?c=15&amp;pt=17</t>
+  </si>
+  <si>
+    <t>AWS Management Console</t>
+  </si>
+  <si>
+    <t>Web-based user interface</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/console/?c=15&amp;pt=16</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/opsworks/?c=15&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/premiumsupport/phd/?c=15&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/servicecatalog/?c=15&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/systems-manager/?c=15&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/trustedadvisor/?c=15&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/well-architected-tool/?c=15&amp;pt=13</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudwatch/?c=15&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediaconnect/?c=16&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediaconvert/?c=16&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/medialive/?c=16&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediapackage/?c=16&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediastore/?c=16&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/mediatailor/?c=16&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/elastictranscoder/?c=16&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kinesis/video-streams/?c=16&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/application-discovery/?c=17&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/datasync/?c=17&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dms/?c=17&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/migration-hub/?c=17&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/server-migration-service/?c=17&amp;pt=4</t>
+  </si>
+  <si>
+    <t>AWS Snowball Family</t>
+  </si>
+  <si>
+    <t>Physical devices to migrate data into and out of AWS</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snow/?c=17&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sftp/?c=17&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/amplify/?c=18&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/appsync/?c=18&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/device-farm/?c=18&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/api-gateway/?c=18&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/pinpoint/?c=18&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/app-mesh/?c=19&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloud-map/?c=19&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/directconnect/?c=19&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/global-accelerator/?c=19&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/transit-gateway/?c=19&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/api-gateway/?c=19&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudfront/?c=19&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/route53/?c=19&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/vpc/?c=19&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/privatelink/?c=19&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/robomaker/?c=20&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ground-station/?c=21&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/artifact/?c=22&amp;pt=17</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/certificate-manager/?c=22&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloudhsm/?c=22&amp;pt=9</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/directoryservice/?c=22&amp;pt=10</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/firewall-manager/?c=22&amp;pt=11</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/iam/?c=22&amp;pt=1</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/kms/?c=22&amp;pt=12</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/organizations/?c=22&amp;pt=13</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/secrets-manager/?c=22&amp;pt=14</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/security-hub/?c=22&amp;pt=18</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/shield/?c=22&amp;pt=15</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/single-sign-on/?c=22&amp;pt=4</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/waf/?c=22&amp;pt=16</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cloud-directory/?c=22&amp;pt=2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/cognito/?c=22&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/guardduty/?c=22&amp;pt=5</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/inspector/?c=22&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/macie/?c=22&amp;pt=7</t>
+  </si>
+  <si>
+    <t>AWS Snow Family</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/snow/?c=23&amp;pt=6</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/storagegateway/?c=23&amp;pt=5</t>
+  </si>
+  <si>
+    <t>Amazon Elastic Block Store (EBS)</t>
+  </si>
+  <si>
+    <t>EC2 block storage volumes</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ebs/?c=23&amp;pt=2</t>
+  </si>
+  <si>
+    <t>Amazon Elastic File System (EFS)</t>
+  </si>
+  <si>
+    <t>Fully managed file system for EC2</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/efs/?c=23&amp;pt=3</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/fsx/lustre/?c=23&amp;pt=7</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/fsx/windows/?c=23&amp;pt=8</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/glacier1/?c=23&amp;pt=4</t>
+  </si>
+  <si>
+    <t>Amazon Simple Storage Service (S3)</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/s3/?c=23&amp;pt=1</t>
   </si>
 </sst>
 </file>
@@ -1683,22 +1716,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1772,8 +1789,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D171" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D171" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D174" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D174" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Product" dataDxfId="2"/>
@@ -2050,10 +2067,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D171"/>
+  <dimension ref="A1:D174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2070,2188 +2087,2188 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>522</v>
+        <v>337</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>232</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>264</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>265</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
+        <v>288</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>266</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
+        <v>134</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>267</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>269</v>
+        <v>138</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>270</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>271</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>272</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>233</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>273</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>289</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>290</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>274</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>275</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>276</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>239</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>277</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>350</v>
       </c>
       <c r="C14" t="s">
-        <v>227</v>
+        <v>351</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>278</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>181</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>179</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>174</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>177</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>173</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>282</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>319</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>320</v>
       </c>
       <c r="C19" t="s">
-        <v>229</v>
+        <v>321</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>283</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>319</v>
       </c>
       <c r="B20" t="s">
-        <v>230</v>
+        <v>322</v>
       </c>
       <c r="C20" t="s">
-        <v>231</v>
+        <v>323</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>284</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>319</v>
       </c>
       <c r="B21" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="C21" t="s">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>287</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>319</v>
       </c>
       <c r="B22" t="s">
-        <v>288</v>
+        <v>326</v>
       </c>
       <c r="C22" t="s">
-        <v>289</v>
+        <v>327</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>290</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>328</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>329</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>330</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>232</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>328</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>256</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>291</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>234</v>
+        <v>308</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>186</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>241</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>292</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>234</v>
+        <v>308</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>187</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>242</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>293</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>234</v>
+        <v>308</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>243</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>294</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>234</v>
+        <v>308</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>189</v>
       </c>
       <c r="C28" t="s">
-        <v>295</v>
+        <v>244</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>296</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>297</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>298</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>299</v>
+        <v>18</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>300</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>217</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>301</v>
+        <v>369</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>302</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>303</v>
+        <v>218</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>304</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>248</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>249</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>305</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>306</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>307</v>
+        <v>22</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>308</v>
+        <v>372</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>235</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>310</v>
+        <v>373</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>311</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>312</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>313</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>314</v>
+        <v>375</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>315</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>236</v>
+        <v>10</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>316</v>
+        <v>377</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>317</v>
+        <v>378</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>224</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>379</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>219</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>319</v>
+        <v>381</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>309</v>
+        <v>182</v>
       </c>
       <c r="B43" t="s">
-        <v>320</v>
+        <v>183</v>
       </c>
       <c r="C43" t="s">
-        <v>321</v>
+        <v>240</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>322</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>182</v>
       </c>
       <c r="B44" t="s">
-        <v>323</v>
+        <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>324</v>
+        <v>168</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>325</v>
+        <v>383</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>182</v>
       </c>
       <c r="B45" t="s">
-        <v>326</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
-        <v>327</v>
+        <v>185</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>328</v>
+        <v>384</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>329</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B47" t="s">
-        <v>330</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>331</v>
+        <v>31</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>332</v>
+        <v>386</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B48" t="s">
-        <v>333</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>334</v>
+        <v>35</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>335</v>
+        <v>387</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
+        <v>254</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>336</v>
+        <v>388</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>337</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>255</v>
       </c>
       <c r="C51" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>338</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>339</v>
+        <v>391</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B53" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="C53" t="s">
-        <v>340</v>
+        <v>258</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>341</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="B54" t="s">
-        <v>238</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>239</v>
+        <v>38</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>342</v>
+        <v>393</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>259</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>260</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>343</v>
+        <v>394</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>192</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>245</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>344</v>
+        <v>395</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>191</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>246</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>345</v>
+        <v>396</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>240</v>
+        <v>68</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>346</v>
+        <v>397</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" t="s">
         <v>63</v>
       </c>
-      <c r="B59" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" t="s">
-        <v>72</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>347</v>
+        <v>398</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>348</v>
+        <v>399</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>225</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>349</v>
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>350</v>
+        <v>401</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>351</v>
+        <v>57</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>352</v>
+        <v>402</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>351</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>353</v>
+        <v>403</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>351</v>
+        <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>404</v>
       </c>
       <c r="C65" t="s">
-        <v>86</v>
+        <v>405</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>354</v>
+        <v>406</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>351</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>355</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>351</v>
+        <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>356</v>
+        <v>408</v>
       </c>
       <c r="C67" t="s">
-        <v>357</v>
+        <v>409</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>358</v>
+        <v>410</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>351</v>
+        <v>411</v>
       </c>
       <c r="B68" t="s">
-        <v>359</v>
+        <v>209</v>
       </c>
       <c r="C68" t="s">
-        <v>360</v>
+        <v>247</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>361</v>
+        <v>412</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>351</v>
+        <v>411</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>210</v>
       </c>
       <c r="C69" t="s">
-        <v>241</v>
+        <v>318</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>362</v>
+        <v>413</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="C70" t="s">
-        <v>242</v>
+        <v>199</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>363</v>
+        <v>414</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="B71" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="C71" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>364</v>
+        <v>415</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>365</v>
+        <v>416</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>204</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>366</v>
+        <v>417</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="B74" t="s">
-        <v>367</v>
+        <v>194</v>
       </c>
       <c r="C74" t="s">
-        <v>368</v>
+        <v>195</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>369</v>
+        <v>418</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>351</v>
+        <v>193</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>206</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>309</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>370</v>
+        <v>419</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="B76" t="s">
-        <v>371</v>
+        <v>207</v>
       </c>
       <c r="C76" t="s">
-        <v>372</v>
+        <v>208</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>373</v>
+        <v>420</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>310</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>311</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>374</v>
+        <v>421</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
+        <v>312</v>
       </c>
       <c r="C78" t="s">
-        <v>105</v>
+        <v>313</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>375</v>
+        <v>422</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="B79" t="s">
-        <v>106</v>
+        <v>314</v>
       </c>
       <c r="C79" t="s">
-        <v>107</v>
+        <v>315</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>376</v>
+        <v>423</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="B80" t="s">
-        <v>108</v>
+        <v>316</v>
       </c>
       <c r="C80" t="s">
-        <v>109</v>
+        <v>317</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>377</v>
+        <v>424</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>97</v>
+        <v>193</v>
       </c>
       <c r="B81" t="s">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>197</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>378</v>
+        <v>425</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
+        <v>235</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>379</v>
+        <v>426</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="B83" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="C83" t="s">
-        <v>101</v>
+        <v>162</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>380</v>
+        <v>427</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
-        <v>243</v>
+        <v>291</v>
       </c>
       <c r="C84" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>381</v>
+        <v>428</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B85" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="C85" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>382</v>
+        <v>429</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>293</v>
       </c>
       <c r="C86" t="s">
-        <v>127</v>
+        <v>294</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>383</v>
+        <v>430</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>295</v>
       </c>
       <c r="C87" t="s">
-        <v>129</v>
+        <v>296</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>384</v>
+        <v>431</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B88" t="s">
-        <v>220</v>
+        <v>297</v>
       </c>
       <c r="C88" t="s">
-        <v>221</v>
+        <v>298</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>385</v>
+        <v>432</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B89" t="s">
-        <v>245</v>
+        <v>151</v>
       </c>
       <c r="C89" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>386</v>
+        <v>433</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B90" t="s">
-        <v>130</v>
+        <v>299</v>
       </c>
       <c r="C90" t="s">
-        <v>131</v>
+        <v>300</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>387</v>
+        <v>434</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B91" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="C91" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>388</v>
+        <v>435</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
+        <v>155</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>156</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>389</v>
+        <v>436</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B93" t="s">
-        <v>390</v>
+        <v>147</v>
       </c>
       <c r="C93" t="s">
-        <v>391</v>
+        <v>148</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>392</v>
+        <v>437</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B94" t="s">
-        <v>134</v>
+        <v>301</v>
       </c>
       <c r="C94" t="s">
-        <v>135</v>
+        <v>302</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>393</v>
+        <v>438</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B95" t="s">
-        <v>117</v>
+        <v>303</v>
       </c>
       <c r="C95" t="s">
-        <v>118</v>
+        <v>304</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>394</v>
+        <v>439</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B96" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="C96" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>395</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="C97" t="s">
-        <v>246</v>
+        <v>158</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>396</v>
+        <v>441</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B98" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="C98" t="s">
-        <v>116</v>
+        <v>236</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>397</v>
+        <v>442</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="B99" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="C99" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>398</v>
+        <v>443</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>112</v>
+        <v>275</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="C100" t="s">
-        <v>122</v>
+        <v>76</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>399</v>
+        <v>444</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>112</v>
+        <v>275</v>
       </c>
       <c r="B101" t="s">
-        <v>123</v>
+        <v>77</v>
       </c>
       <c r="C101" t="s">
-        <v>400</v>
+        <v>78</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>401</v>
+        <v>445</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B102" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="C102" t="s">
-        <v>247</v>
+        <v>80</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>402</v>
+        <v>446</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B103" t="s">
-        <v>150</v>
+        <v>71</v>
       </c>
       <c r="C103" t="s">
-        <v>151</v>
+        <v>447</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>403</v>
+        <v>448</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B104" t="s">
-        <v>404</v>
+        <v>81</v>
       </c>
       <c r="C104" t="s">
-        <v>405</v>
+        <v>82</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>406</v>
+        <v>449</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B105" t="s">
-        <v>139</v>
+        <v>450</v>
       </c>
       <c r="C105" t="s">
-        <v>140</v>
+        <v>451</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>407</v>
+        <v>452</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B106" t="s">
-        <v>143</v>
+        <v>276</v>
       </c>
       <c r="C106" t="s">
-        <v>144</v>
+        <v>277</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>408</v>
+        <v>453</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B107" t="s">
-        <v>141</v>
+        <v>278</v>
       </c>
       <c r="C107" t="s">
-        <v>142</v>
+        <v>279</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>409</v>
+        <v>454</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B108" t="s">
-        <v>145</v>
+        <v>455</v>
       </c>
       <c r="C108" t="s">
-        <v>146</v>
+        <v>456</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>410</v>
+        <v>457</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B109" t="s">
-        <v>147</v>
+        <v>458</v>
       </c>
       <c r="C109" t="s">
-        <v>248</v>
+        <v>459</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>411</v>
+        <v>460</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B110" t="s">
-        <v>412</v>
+        <v>83</v>
       </c>
       <c r="C110" t="s">
-        <v>413</v>
+        <v>226</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>414</v>
+        <v>461</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B111" t="s">
-        <v>249</v>
+        <v>90</v>
       </c>
       <c r="C111" t="s">
-        <v>148</v>
+        <v>227</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>415</v>
+        <v>462</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B112" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C112" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>416</v>
+        <v>463</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>152</v>
+        <v>275</v>
       </c>
       <c r="B113" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
       <c r="C113" t="s">
-        <v>250</v>
+        <v>87</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>417</v>
+        <v>464</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>152</v>
+        <v>275</v>
       </c>
       <c r="B114" t="s">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="C114" t="s">
-        <v>168</v>
+        <v>89</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>418</v>
+        <v>465</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>152</v>
+        <v>275</v>
       </c>
       <c r="B115" t="s">
-        <v>419</v>
+        <v>280</v>
       </c>
       <c r="C115" t="s">
-        <v>420</v>
+        <v>281</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>421</v>
+        <v>466</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>152</v>
+        <v>275</v>
       </c>
       <c r="B116" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="C116" t="s">
-        <v>156</v>
+        <v>74</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>422</v>
+        <v>467</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B117" t="s">
-        <v>423</v>
+        <v>282</v>
       </c>
       <c r="C117" t="s">
-        <v>424</v>
+        <v>283</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>425</v>
+        <v>468</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B118" t="s">
-        <v>426</v>
+        <v>96</v>
       </c>
       <c r="C118" t="s">
-        <v>427</v>
+        <v>97</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>428</v>
+        <v>469</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B119" t="s">
-        <v>429</v>
+        <v>98</v>
       </c>
       <c r="C119" t="s">
-        <v>430</v>
+        <v>99</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>431</v>
+        <v>470</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B120" t="s">
-        <v>157</v>
+        <v>100</v>
       </c>
       <c r="C120" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>432</v>
+        <v>471</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B121" t="s">
-        <v>433</v>
+        <v>102</v>
       </c>
       <c r="C121" t="s">
-        <v>434</v>
+        <v>103</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>435</v>
+        <v>472</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B122" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="C122" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>436</v>
+        <v>473</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B123" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
       <c r="C123" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="B124" t="s">
-        <v>153</v>
+        <v>94</v>
       </c>
       <c r="C124" t="s">
-        <v>154</v>
+        <v>95</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>438</v>
+        <v>475</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>152</v>
+        <v>261</v>
       </c>
       <c r="B125" t="s">
-        <v>439</v>
+        <v>43</v>
       </c>
       <c r="C125" t="s">
-        <v>440</v>
+        <v>221</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>441</v>
+        <v>476</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>152</v>
+        <v>261</v>
       </c>
       <c r="B126" t="s">
-        <v>442</v>
+        <v>262</v>
       </c>
       <c r="C126" t="s">
-        <v>443</v>
+        <v>263</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>444</v>
+        <v>477</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>152</v>
+        <v>261</v>
       </c>
       <c r="B127" t="s">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="C127" t="s">
-        <v>166</v>
+        <v>42</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>445</v>
+        <v>478</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>152</v>
+        <v>261</v>
       </c>
       <c r="B128" t="s">
-        <v>163</v>
+        <v>44</v>
       </c>
       <c r="C128" t="s">
-        <v>164</v>
+        <v>45</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>446</v>
+        <v>479</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>152</v>
+        <v>261</v>
       </c>
       <c r="B129" t="s">
-        <v>170</v>
+        <v>46</v>
       </c>
       <c r="C129" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>447</v>
+        <v>480</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>152</v>
+        <v>261</v>
       </c>
       <c r="B130" t="s">
-        <v>171</v>
+        <v>481</v>
       </c>
       <c r="C130" t="s">
-        <v>172</v>
+        <v>482</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>448</v>
+        <v>483</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>449</v>
+        <v>261</v>
       </c>
       <c r="B131" t="s">
-        <v>450</v>
+        <v>264</v>
       </c>
       <c r="C131" t="s">
-        <v>451</v>
+        <v>265</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>452</v>
+        <v>484</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>449</v>
+        <v>305</v>
       </c>
       <c r="B132" t="s">
-        <v>175</v>
+        <v>306</v>
       </c>
       <c r="C132" t="s">
-        <v>252</v>
+        <v>307</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>453</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>449</v>
+        <v>305</v>
       </c>
       <c r="B133" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C133" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>454</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>449</v>
+        <v>305</v>
       </c>
       <c r="B134" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C134" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>455</v>
+        <v>487</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>449</v>
+        <v>305</v>
       </c>
       <c r="B135" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C135" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>456</v>
+        <v>488</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>449</v>
+        <v>305</v>
       </c>
       <c r="B136" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C136" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>457</v>
+        <v>489</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>178</v>
+        <v>47</v>
       </c>
       <c r="B137" t="s">
-        <v>179</v>
+        <v>266</v>
       </c>
       <c r="C137" t="s">
-        <v>180</v>
+        <v>267</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>458</v>
+        <v>490</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>181</v>
+        <v>47</v>
       </c>
       <c r="B138" t="s">
-        <v>182</v>
+        <v>268</v>
       </c>
       <c r="C138" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>459</v>
+        <v>491</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>181</v>
+        <v>47</v>
       </c>
       <c r="B139" t="s">
-        <v>187</v>
+        <v>55</v>
       </c>
       <c r="C139" t="s">
-        <v>188</v>
+        <v>56</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>460</v>
+        <v>492</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>181</v>
+        <v>47</v>
       </c>
       <c r="B140" t="s">
-        <v>185</v>
+        <v>270</v>
       </c>
       <c r="C140" t="s">
-        <v>186</v>
+        <v>271</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>461</v>
+        <v>493</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>181</v>
+        <v>47</v>
       </c>
       <c r="B141" t="s">
-        <v>183</v>
+        <v>272</v>
       </c>
       <c r="C141" t="s">
-        <v>184</v>
+        <v>273</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>462</v>
+        <v>494</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>189</v>
+        <v>47</v>
       </c>
       <c r="B142" t="s">
-        <v>190</v>
+        <v>53</v>
       </c>
       <c r="C142" t="s">
-        <v>256</v>
+        <v>54</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>463</v>
+        <v>495</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>189</v>
+        <v>47</v>
       </c>
       <c r="B143" t="s">
-        <v>173</v>
+        <v>50</v>
       </c>
       <c r="C143" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>464</v>
+        <v>496</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>189</v>
+        <v>47</v>
       </c>
       <c r="B144" t="s">
-        <v>191</v>
+        <v>52</v>
       </c>
       <c r="C144" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>465</v>
+        <v>497</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>466</v>
+        <v>47</v>
       </c>
       <c r="B145" t="s">
-        <v>193</v>
+        <v>48</v>
       </c>
       <c r="C145" t="s">
-        <v>257</v>
+        <v>49</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>467</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>466</v>
+        <v>47</v>
       </c>
       <c r="B146" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="C146" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>466</v>
+        <v>331</v>
       </c>
       <c r="B147" t="s">
-        <v>195</v>
+        <v>332</v>
       </c>
       <c r="C147" t="s">
-        <v>259</v>
+        <v>333</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>469</v>
+        <v>500</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>466</v>
+        <v>334</v>
       </c>
       <c r="B148" t="s">
-        <v>196</v>
+        <v>335</v>
       </c>
       <c r="C148" t="s">
-        <v>260</v>
+        <v>336</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>197</v>
+        <v>106</v>
       </c>
       <c r="B149" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="C149" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>471</v>
+        <v>502</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>197</v>
+        <v>106</v>
       </c>
       <c r="B150" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="C150" t="s">
-        <v>262</v>
+        <v>119</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>472</v>
+        <v>503</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B151" t="s">
-        <v>205</v>
+        <v>120</v>
       </c>
       <c r="C151" t="s">
-        <v>206</v>
+        <v>121</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>473</v>
+        <v>504</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B152" t="s">
-        <v>207</v>
+        <v>122</v>
       </c>
       <c r="C152" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B153" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C153" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>475</v>
+        <v>506</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B154" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="C154" t="s">
-        <v>212</v>
+        <v>107</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B155" t="s">
-        <v>201</v>
+        <v>124</v>
       </c>
       <c r="C155" t="s">
-        <v>202</v>
+        <v>125</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>477</v>
+        <v>508</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B156" t="s">
-        <v>213</v>
+        <v>126</v>
       </c>
       <c r="C156" t="s">
-        <v>478</v>
+        <v>127</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>479</v>
+        <v>509</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B157" t="s">
         <v>214</v>
@@ -4260,203 +4277,245 @@
         <v>215</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>480</v>
+        <v>510</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B158" t="s">
-        <v>481</v>
+        <v>284</v>
       </c>
       <c r="C158" t="s">
-        <v>482</v>
+        <v>285</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>483</v>
+        <v>511</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B159" t="s">
-        <v>484</v>
+        <v>128</v>
       </c>
       <c r="C159" t="s">
-        <v>485</v>
+        <v>129</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>486</v>
+        <v>512</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B160" t="s">
-        <v>487</v>
+        <v>111</v>
       </c>
       <c r="C160" t="s">
-        <v>488</v>
+        <v>112</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>489</v>
+        <v>513</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B161" t="s">
-        <v>490</v>
+        <v>130</v>
       </c>
       <c r="C161" t="s">
-        <v>491</v>
+        <v>131</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>492</v>
+        <v>514</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B162" t="s">
-        <v>203</v>
+        <v>108</v>
       </c>
       <c r="C162" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>493</v>
+        <v>515</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>216</v>
+        <v>106</v>
       </c>
       <c r="B163" t="s">
-        <v>217</v>
+        <v>109</v>
       </c>
       <c r="C163" t="s">
-        <v>263</v>
+        <v>110</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>494</v>
+        <v>516</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>216</v>
+        <v>106</v>
       </c>
       <c r="B164" t="s">
-        <v>218</v>
+        <v>113</v>
       </c>
       <c r="C164" t="s">
-        <v>495</v>
+        <v>114</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>496</v>
+        <v>517</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>497</v>
+        <v>106</v>
       </c>
       <c r="B165" t="s">
-        <v>498</v>
+        <v>115</v>
       </c>
       <c r="C165" t="s">
-        <v>499</v>
+        <v>116</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>497</v>
+        <v>106</v>
       </c>
       <c r="B166" t="s">
-        <v>501</v>
+        <v>117</v>
       </c>
       <c r="C166" t="s">
-        <v>502</v>
+        <v>286</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>497</v>
+        <v>24</v>
       </c>
       <c r="B167" t="s">
-        <v>504</v>
+        <v>520</v>
       </c>
       <c r="C167" t="s">
-        <v>505</v>
+        <v>482</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>506</v>
+        <v>521</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>497</v>
+        <v>24</v>
       </c>
       <c r="B168" t="s">
-        <v>507</v>
+        <v>28</v>
       </c>
       <c r="C168" t="s">
-        <v>508</v>
+        <v>29</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>509</v>
+        <v>522</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>510</v>
+        <v>24</v>
       </c>
       <c r="B169" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="C169" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>514</v>
+        <v>24</v>
       </c>
       <c r="B170" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="C170" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>518</v>
+        <v>24</v>
       </c>
       <c r="B171" t="s">
-        <v>519</v>
+        <v>250</v>
       </c>
       <c r="C171" t="s">
-        <v>520</v>
+        <v>251</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>521</v>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>24</v>
+      </c>
+      <c r="B172" t="s">
+        <v>252</v>
+      </c>
+      <c r="C172" t="s">
+        <v>253</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>24</v>
+      </c>
+      <c r="B173" t="s">
+        <v>26</v>
+      </c>
+      <c r="C173" t="s">
+        <v>27</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>24</v>
+      </c>
+      <c r="B174" t="s">
+        <v>532</v>
+      </c>
+      <c r="C174" t="s">
+        <v>25</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>